<commit_message>
fix adding attributions, run the scripts and output new files
</commit_message>
<xml_diff>
--- a/WD_BDRC_data.xlsx
+++ b/WD_BDRC_data.xlsx
@@ -716,7 +716,7 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
@@ -757,7 +757,7 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
       <c r="M7" t="inlineStr"/>
@@ -847,7 +847,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
@@ -892,7 +892,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M10" t="inlineStr"/>
@@ -982,7 +982,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M12" t="inlineStr"/>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M13" t="inlineStr"/>
@@ -1072,7 +1072,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M14" t="inlineStr"/>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M15" t="inlineStr"/>
@@ -1162,7 +1162,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M16" t="inlineStr"/>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M19" t="inlineStr"/>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M20" t="inlineStr"/>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M22" t="inlineStr"/>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M23" t="inlineStr"/>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M25" t="inlineStr"/>
@@ -1612,7 +1612,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M26" t="inlineStr"/>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M28" t="inlineStr"/>
@@ -1792,7 +1792,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M30" t="inlineStr"/>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M40" t="inlineStr"/>
@@ -2316,7 +2316,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M42" t="inlineStr"/>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M43" t="inlineStr"/>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M44" t="inlineStr"/>
@@ -2451,7 +2451,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M45" t="inlineStr"/>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M47" t="inlineStr"/>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M48" t="inlineStr"/>
@@ -2676,7 +2676,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M50" t="inlineStr"/>
@@ -2721,7 +2721,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M51" t="inlineStr"/>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M52" t="inlineStr"/>
@@ -2811,7 +2811,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M53" t="inlineStr"/>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M54" t="inlineStr"/>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M56" t="inlineStr"/>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M59" t="inlineStr"/>
@@ -3204,7 +3204,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M62" t="inlineStr"/>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M63" t="inlineStr"/>
@@ -3339,7 +3339,7 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M65" t="inlineStr"/>
@@ -3429,7 +3429,7 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M67" t="inlineStr"/>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M69" t="inlineStr"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M71" t="inlineStr"/>
@@ -3654,7 +3654,7 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M72" t="inlineStr"/>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M73" t="inlineStr"/>
@@ -3744,7 +3744,7 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M74" t="inlineStr"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M75" t="inlineStr"/>
@@ -3834,7 +3834,7 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M76" t="inlineStr"/>
@@ -3879,7 +3879,7 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M77" t="inlineStr"/>
@@ -3924,7 +3924,7 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M78" t="inlineStr"/>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M79" t="inlineStr"/>
@@ -4014,7 +4014,7 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M80" t="inlineStr"/>
@@ -4149,7 +4149,7 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M83" t="inlineStr"/>
@@ -4194,7 +4194,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M84" t="inlineStr"/>
@@ -4239,7 +4239,7 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M85" t="inlineStr"/>
@@ -4284,7 +4284,7 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M86" t="inlineStr"/>
@@ -4419,7 +4419,7 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M89" t="inlineStr"/>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M91" t="inlineStr"/>
@@ -4550,7 +4550,7 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M92" t="inlineStr"/>
@@ -4636,7 +4636,7 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M94" t="inlineStr"/>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M97" t="inlineStr"/>
@@ -5246,7 +5246,7 @@
       </c>
       <c r="L108" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M108" t="inlineStr"/>
@@ -5471,7 +5471,7 @@
       </c>
       <c r="L113" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M113" t="inlineStr"/>
@@ -5606,7 +5606,7 @@
       </c>
       <c r="L116" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M116" t="inlineStr"/>
@@ -5651,7 +5651,7 @@
       </c>
       <c r="L117" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M117" t="inlineStr"/>
@@ -5782,7 +5782,7 @@
       </c>
       <c r="L120" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M120" t="inlineStr"/>
@@ -5827,7 +5827,7 @@
       </c>
       <c r="L121" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M121" t="inlineStr"/>
@@ -5913,7 +5913,7 @@
       </c>
       <c r="L123" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M123" t="inlineStr"/>
@@ -6003,7 +6003,7 @@
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M125" t="inlineStr"/>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M127" t="inlineStr"/>
@@ -6138,7 +6138,7 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M128" t="inlineStr"/>
@@ -6183,7 +6183,7 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
       <c r="M129" t="inlineStr"/>
@@ -6269,7 +6269,7 @@
       </c>
       <c r="L131" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M131" t="inlineStr"/>
@@ -6494,7 +6494,7 @@
       </c>
       <c r="L136" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M136" t="inlineStr"/>
@@ -6539,7 +6539,7 @@
       </c>
       <c r="L137" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M137" t="inlineStr"/>
@@ -6584,7 +6584,7 @@
       </c>
       <c r="L138" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M138" t="inlineStr"/>
@@ -6674,7 +6674,7 @@
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M140" t="inlineStr"/>
@@ -6719,7 +6719,7 @@
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M141" t="inlineStr"/>
@@ -6764,7 +6764,7 @@
       </c>
       <c r="L142" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M142" t="inlineStr"/>
@@ -6809,7 +6809,7 @@
       </c>
       <c r="L143" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M143" t="inlineStr"/>
@@ -6854,7 +6854,7 @@
       </c>
       <c r="L144" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M144" t="inlineStr"/>
@@ -6899,7 +6899,7 @@
       </c>
       <c r="L145" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M145" t="inlineStr"/>
@@ -6944,7 +6944,7 @@
       </c>
       <c r="L146" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M146" t="inlineStr"/>
@@ -6989,7 +6989,7 @@
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M147" t="inlineStr"/>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="L149" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M149" t="inlineStr"/>
@@ -7120,7 +7120,7 @@
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M150" t="inlineStr"/>
@@ -7210,7 +7210,7 @@
       </c>
       <c r="L152" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M152" t="inlineStr"/>
@@ -7300,7 +7300,7 @@
       </c>
       <c r="L154" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M154" t="inlineStr"/>
@@ -7345,7 +7345,7 @@
       </c>
       <c r="L155" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M155" t="inlineStr"/>
@@ -7390,7 +7390,7 @@
       </c>
       <c r="L156" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M156" t="inlineStr"/>
@@ -7480,7 +7480,7 @@
       </c>
       <c r="L158" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M158" t="inlineStr"/>
@@ -7525,7 +7525,7 @@
       </c>
       <c r="L159" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M159" t="inlineStr"/>
@@ -7701,7 +7701,7 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M163" t="inlineStr"/>
@@ -7746,7 +7746,7 @@
       </c>
       <c r="L164" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M164" t="inlineStr"/>
@@ -7877,7 +7877,7 @@
       </c>
       <c r="L167" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M167" t="inlineStr"/>
@@ -7922,7 +7922,7 @@
       </c>
       <c r="L168" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M168" t="inlineStr"/>
@@ -8012,7 +8012,7 @@
       </c>
       <c r="L170" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M170" t="inlineStr"/>
@@ -8057,7 +8057,7 @@
       </c>
       <c r="L171" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M171" t="inlineStr"/>
@@ -8143,7 +8143,7 @@
       </c>
       <c r="L173" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
       <c r="M173" t="inlineStr"/>
@@ -8188,7 +8188,7 @@
       </c>
       <c r="L174" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M174" t="inlineStr"/>
@@ -8278,7 +8278,7 @@
       </c>
       <c r="L176" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M176" t="inlineStr"/>
@@ -8323,7 +8323,7 @@
       </c>
       <c r="L177" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M177" t="inlineStr"/>
@@ -8458,7 +8458,7 @@
       </c>
       <c r="L180" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M180" t="inlineStr"/>
@@ -8503,7 +8503,7 @@
       </c>
       <c r="L181" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M181" t="inlineStr"/>
@@ -8548,7 +8548,7 @@
       </c>
       <c r="L182" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M182" t="inlineStr"/>
@@ -8683,7 +8683,7 @@
       </c>
       <c r="L185" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M185" t="inlineStr"/>
@@ -8818,7 +8818,7 @@
       </c>
       <c r="L188" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M188" t="inlineStr"/>
@@ -8953,7 +8953,7 @@
       </c>
       <c r="L191" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M191" t="inlineStr"/>
@@ -9088,7 +9088,7 @@
       </c>
       <c r="L194" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M194" t="inlineStr"/>
@@ -9178,7 +9178,7 @@
       </c>
       <c r="L196" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M196" t="inlineStr"/>
@@ -9223,7 +9223,7 @@
       </c>
       <c r="L197" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M197" t="inlineStr"/>
@@ -9448,7 +9448,7 @@
       </c>
       <c r="L202" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M202" t="inlineStr"/>
@@ -9493,7 +9493,7 @@
       </c>
       <c r="L203" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M203" t="inlineStr"/>
@@ -9538,7 +9538,7 @@
       </c>
       <c r="L204" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M204" t="inlineStr"/>
@@ -9628,7 +9628,7 @@
       </c>
       <c r="L206" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M206" t="inlineStr"/>
@@ -9673,7 +9673,7 @@
       </c>
       <c r="L207" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M207" t="inlineStr"/>
@@ -9759,7 +9759,7 @@
       </c>
       <c r="L209" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M209" t="inlineStr"/>
@@ -9894,7 +9894,7 @@
       </c>
       <c r="L212" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M212" t="inlineStr"/>
@@ -9939,7 +9939,7 @@
       </c>
       <c r="L213" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M213" t="inlineStr"/>
@@ -10025,7 +10025,7 @@
       </c>
       <c r="L215" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M215" t="inlineStr"/>
@@ -10295,7 +10295,7 @@
       </c>
       <c r="L221" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M221" t="inlineStr"/>
@@ -10340,7 +10340,7 @@
       </c>
       <c r="L222" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M222" t="inlineStr"/>
@@ -10430,7 +10430,7 @@
       </c>
       <c r="L224" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M224" t="inlineStr"/>
@@ -10520,7 +10520,7 @@
       </c>
       <c r="L226" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M226" t="inlineStr"/>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="L229" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M229" t="inlineStr"/>
@@ -10700,7 +10700,7 @@
       </c>
       <c r="L230" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M230" t="inlineStr"/>
@@ -10790,7 +10790,7 @@
       </c>
       <c r="L232" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M232" t="inlineStr"/>
@@ -10880,7 +10880,7 @@
       </c>
       <c r="L234" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M234" t="inlineStr"/>
@@ -10925,7 +10925,7 @@
       </c>
       <c r="L235" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M235" t="inlineStr"/>
@@ -11015,7 +11015,7 @@
       </c>
       <c r="L237" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M237" t="inlineStr"/>
@@ -11105,7 +11105,7 @@
       </c>
       <c r="L239" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M239" t="inlineStr"/>
@@ -11461,7 +11461,7 @@
       </c>
       <c r="L247" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M247" t="inlineStr"/>
@@ -11506,7 +11506,7 @@
       </c>
       <c r="L248" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M248" t="inlineStr"/>
@@ -11551,7 +11551,7 @@
       </c>
       <c r="L249" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M249" t="inlineStr"/>
@@ -11596,7 +11596,7 @@
       </c>
       <c r="L250" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M250" t="inlineStr"/>
@@ -11682,7 +11682,7 @@
       </c>
       <c r="L252" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M252" t="inlineStr"/>
@@ -11772,7 +11772,7 @@
       </c>
       <c r="L254" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M254" t="inlineStr"/>
@@ -11862,7 +11862,7 @@
       </c>
       <c r="L256" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M256" t="inlineStr"/>
@@ -11952,7 +11952,7 @@
       </c>
       <c r="L258" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M258" t="inlineStr"/>
@@ -12042,7 +12042,7 @@
       </c>
       <c r="L260" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M260" t="inlineStr"/>
@@ -12169,7 +12169,7 @@
       </c>
       <c r="L263" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M263" t="inlineStr"/>
@@ -12259,7 +12259,7 @@
       </c>
       <c r="L265" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M265" t="inlineStr"/>
@@ -12345,7 +12345,7 @@
       </c>
       <c r="L267" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M267" t="inlineStr"/>
@@ -12435,7 +12435,7 @@
       </c>
       <c r="L269" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M269" t="inlineStr"/>
@@ -12570,7 +12570,7 @@
       </c>
       <c r="L272" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M272" t="inlineStr"/>
@@ -12750,7 +12750,7 @@
       </c>
       <c r="L276" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M276" t="inlineStr"/>
@@ -13106,7 +13106,7 @@
       </c>
       <c r="L284" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M284" t="inlineStr"/>
@@ -13401,7 +13401,7 @@
       </c>
       <c r="L291" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M291" t="inlineStr"/>
@@ -13618,7 +13618,7 @@
       </c>
       <c r="L296" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M296" t="inlineStr"/>
@@ -13704,7 +13704,7 @@
       </c>
       <c r="L298" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M298" t="inlineStr"/>
@@ -13749,7 +13749,7 @@
       </c>
       <c r="L299" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M299" t="inlineStr"/>
@@ -13835,7 +13835,7 @@
       </c>
       <c r="L301" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M301" t="inlineStr"/>
@@ -13880,7 +13880,7 @@
       </c>
       <c r="L302" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M302" t="inlineStr"/>
@@ -13970,7 +13970,7 @@
       </c>
       <c r="L304" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M304" t="inlineStr"/>
@@ -14015,7 +14015,7 @@
       </c>
       <c r="L305" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M305" t="inlineStr"/>
@@ -14101,7 +14101,7 @@
       </c>
       <c r="L307" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M307" t="inlineStr"/>
@@ -14273,7 +14273,7 @@
       </c>
       <c r="L311" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M311" t="inlineStr"/>
@@ -14318,7 +14318,7 @@
       </c>
       <c r="L312" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M312" t="inlineStr"/>
@@ -14363,7 +14363,7 @@
       </c>
       <c r="L313" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M313" t="inlineStr"/>
@@ -14498,7 +14498,7 @@
       </c>
       <c r="L316" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M316" t="inlineStr"/>
@@ -14588,7 +14588,7 @@
       </c>
       <c r="L318" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M318" t="inlineStr"/>
@@ -14723,7 +14723,7 @@
       </c>
       <c r="L321" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M321" t="inlineStr"/>
@@ -14768,7 +14768,7 @@
       </c>
       <c r="L322" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
       <c r="M322" t="inlineStr"/>
@@ -14813,7 +14813,7 @@
       </c>
       <c r="L323" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M323" t="inlineStr"/>
@@ -14858,7 +14858,7 @@
       </c>
       <c r="L324" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M324" t="inlineStr"/>
@@ -14944,7 +14944,7 @@
       </c>
       <c r="L326" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M326" t="inlineStr"/>
@@ -14989,7 +14989,7 @@
       </c>
       <c r="L327" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M327" t="inlineStr"/>
@@ -15034,7 +15034,7 @@
       </c>
       <c r="L328" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
       <c r="M328" t="inlineStr"/>
@@ -15079,7 +15079,7 @@
       </c>
       <c r="L329" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M329" t="inlineStr"/>
@@ -15169,7 +15169,7 @@
       </c>
       <c r="L331" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M331" t="inlineStr"/>
@@ -15304,7 +15304,7 @@
       </c>
       <c r="L334" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M334" t="inlineStr"/>
@@ -15349,7 +15349,7 @@
       </c>
       <c r="L335" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
       <c r="M335" t="inlineStr"/>
@@ -15394,7 +15394,7 @@
       </c>
       <c r="L336" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M336" t="inlineStr"/>
@@ -15574,7 +15574,7 @@
       </c>
       <c r="L340" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M340" t="inlineStr"/>
@@ -15664,7 +15664,7 @@
       </c>
       <c r="L342" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M342" t="inlineStr"/>
@@ -15709,7 +15709,7 @@
       </c>
       <c r="L343" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M343" t="inlineStr"/>
@@ -15799,7 +15799,7 @@
       </c>
       <c r="L345" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M345" t="inlineStr"/>
@@ -15844,7 +15844,7 @@
       </c>
       <c r="L346" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M346" t="inlineStr"/>
@@ -15889,7 +15889,7 @@
       </c>
       <c r="L347" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M347" t="inlineStr"/>
@@ -15934,7 +15934,7 @@
       </c>
       <c r="L348" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M348" t="inlineStr"/>
@@ -16065,7 +16065,7 @@
       </c>
       <c r="L351" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M351" t="inlineStr"/>
@@ -16110,7 +16110,7 @@
       </c>
       <c r="L352" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M352" t="inlineStr"/>
@@ -16245,7 +16245,7 @@
       </c>
       <c r="L355" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M355" t="inlineStr"/>
@@ -16331,7 +16331,7 @@
       </c>
       <c r="L357" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
       <c r="M357" t="inlineStr"/>
@@ -16376,7 +16376,7 @@
       </c>
       <c r="L358" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M358" t="inlineStr"/>
@@ -16511,7 +16511,7 @@
       </c>
       <c r="L361" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M361" t="inlineStr"/>
@@ -16601,7 +16601,7 @@
       </c>
       <c r="L363" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M363" t="inlineStr"/>
@@ -16646,7 +16646,7 @@
       </c>
       <c r="L364" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M364" t="inlineStr"/>
@@ -16732,7 +16732,7 @@
       </c>
       <c r="L366" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M366" t="inlineStr"/>
@@ -16777,7 +16777,7 @@
       </c>
       <c r="L367" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M367" t="inlineStr"/>
@@ -16863,7 +16863,7 @@
       </c>
       <c r="L369" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M369" t="inlineStr"/>
@@ -17080,7 +17080,7 @@
       </c>
       <c r="L374" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M374" t="inlineStr"/>
@@ -17125,7 +17125,7 @@
       </c>
       <c r="L375" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M375" t="inlineStr"/>
@@ -17215,7 +17215,7 @@
       </c>
       <c r="L377" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M377" t="inlineStr"/>
@@ -17260,7 +17260,7 @@
       </c>
       <c r="L378" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
       <c r="M378" t="inlineStr"/>
@@ -17481,7 +17481,7 @@
       </c>
       <c r="L383" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M383" t="inlineStr"/>
@@ -17526,7 +17526,7 @@
       </c>
       <c r="L384" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M384" t="inlineStr"/>
@@ -17612,7 +17612,7 @@
       </c>
       <c r="L386" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
       <c r="M386" t="inlineStr"/>
@@ -17657,7 +17657,7 @@
       </c>
       <c r="L387" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M387" t="inlineStr"/>
@@ -17923,7 +17923,7 @@
       </c>
       <c r="L393" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M393" t="inlineStr"/>
@@ -18013,7 +18013,7 @@
       </c>
       <c r="L395" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M395" t="inlineStr"/>
@@ -18103,7 +18103,7 @@
       </c>
       <c r="L397" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M397" t="inlineStr"/>
@@ -18148,7 +18148,7 @@
       </c>
       <c r="L398" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M398" t="inlineStr"/>
@@ -18234,7 +18234,7 @@
       </c>
       <c r="L400" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M400" t="inlineStr"/>
@@ -18361,7 +18361,7 @@
       </c>
       <c r="L403" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M403" t="inlineStr"/>
@@ -18406,7 +18406,7 @@
       </c>
       <c r="L404" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M404" t="inlineStr"/>
@@ -18496,7 +18496,7 @@
       </c>
       <c r="L406" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M406" t="inlineStr"/>
@@ -18541,7 +18541,7 @@
       </c>
       <c r="L407" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M407" t="inlineStr"/>
@@ -18631,7 +18631,7 @@
       </c>
       <c r="L409" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M409" t="inlineStr"/>
@@ -18721,7 +18721,7 @@
       </c>
       <c r="L411" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M411" t="inlineStr"/>
@@ -18811,7 +18811,7 @@
       </c>
       <c r="L413" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M413" t="inlineStr"/>
@@ -18901,7 +18901,7 @@
       </c>
       <c r="L415" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M415" t="inlineStr"/>
@@ -18946,7 +18946,7 @@
       </c>
       <c r="L416" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M416" t="inlineStr"/>
@@ -18991,7 +18991,7 @@
       </c>
       <c r="L417" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M417" t="inlineStr"/>
@@ -19081,7 +19081,7 @@
       </c>
       <c r="L419" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M419" t="inlineStr"/>
@@ -19171,7 +19171,7 @@
       </c>
       <c r="L421" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M421" t="inlineStr"/>
@@ -19216,7 +19216,7 @@
       </c>
       <c r="L422" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M422" t="inlineStr"/>
@@ -19306,7 +19306,7 @@
       </c>
       <c r="L424" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M424" t="inlineStr"/>
@@ -19351,7 +19351,7 @@
       </c>
       <c r="L425" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M425" t="inlineStr"/>
@@ -19441,7 +19441,7 @@
       </c>
       <c r="L427" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M427" t="inlineStr"/>
@@ -19486,7 +19486,7 @@
       </c>
       <c r="L428" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M428" t="inlineStr"/>
@@ -19576,7 +19576,7 @@
       </c>
       <c r="L430" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M430" t="inlineStr"/>
@@ -19621,7 +19621,7 @@
       </c>
       <c r="L431" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M431" t="inlineStr"/>
@@ -19711,7 +19711,7 @@
       </c>
       <c r="L433" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M433" t="inlineStr"/>
@@ -19756,7 +19756,7 @@
       </c>
       <c r="L434" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M434" t="inlineStr"/>
@@ -19846,7 +19846,7 @@
       </c>
       <c r="L436" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M436" t="inlineStr"/>
@@ -19932,7 +19932,7 @@
       </c>
       <c r="L438" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M438" t="inlineStr"/>
@@ -20153,7 +20153,7 @@
       </c>
       <c r="L443" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M443" t="inlineStr"/>
@@ -20460,7 +20460,7 @@
       </c>
       <c r="L450" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M450" t="inlineStr"/>
@@ -20595,7 +20595,7 @@
       </c>
       <c r="L453" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M453" t="inlineStr"/>
@@ -20685,7 +20685,7 @@
       </c>
       <c r="L455" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M455" t="inlineStr"/>
@@ -20857,7 +20857,7 @@
       </c>
       <c r="L459" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M459" t="inlineStr"/>
@@ -20947,7 +20947,7 @@
       </c>
       <c r="L461" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M461" t="inlineStr"/>
@@ -20992,7 +20992,7 @@
       </c>
       <c r="L462" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M462" t="inlineStr"/>
@@ -21209,7 +21209,7 @@
       </c>
       <c r="L467" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M467" t="inlineStr"/>
@@ -21254,7 +21254,7 @@
       </c>
       <c r="L468" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M468" t="inlineStr"/>
@@ -21385,7 +21385,7 @@
       </c>
       <c r="L471" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M471" t="inlineStr"/>
@@ -21516,7 +21516,7 @@
       </c>
       <c r="L474" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M474" t="inlineStr"/>
@@ -21688,7 +21688,7 @@
       </c>
       <c r="L478" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M478" t="inlineStr"/>
@@ -21778,7 +21778,7 @@
       </c>
       <c r="L480" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
       <c r="M480" t="inlineStr"/>
@@ -21823,7 +21823,7 @@
       </c>
       <c r="L481" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M481" t="inlineStr"/>
@@ -22085,7 +22085,7 @@
       </c>
       <c r="L487" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M487" t="inlineStr"/>
@@ -22220,7 +22220,7 @@
       </c>
       <c r="L490" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
       <c r="M490" t="inlineStr"/>
@@ -22265,7 +22265,7 @@
       </c>
       <c r="L491" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M491" t="inlineStr"/>
@@ -22310,7 +22310,7 @@
       </c>
       <c r="L492" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M492" t="inlineStr"/>
@@ -22355,7 +22355,7 @@
       </c>
       <c r="L493" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M493" t="inlineStr"/>
@@ -22531,7 +22531,7 @@
       </c>
       <c r="L497" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M497" t="inlineStr"/>
@@ -27389,7 +27389,7 @@
       </c>
       <c r="L611" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M611" t="inlineStr"/>
@@ -31752,7 +31752,7 @@
       </c>
       <c r="L714" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M714" t="inlineStr"/>
@@ -31842,7 +31842,7 @@
       </c>
       <c r="L716" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M716" t="inlineStr"/>
@@ -32059,7 +32059,7 @@
       </c>
       <c r="L721" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M721" t="inlineStr"/>
@@ -32641,7 +32641,7 @@
       </c>
       <c r="L735" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M735" t="inlineStr"/>
@@ -33489,7 +33489,7 @@
       </c>
       <c r="L755" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M755" t="inlineStr"/>
@@ -33575,7 +33575,7 @@
       </c>
       <c r="L757" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
       <c r="M757" t="inlineStr"/>
@@ -33620,7 +33620,7 @@
       </c>
       <c r="L758" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M758" t="inlineStr"/>
@@ -35337,7 +35337,7 @@
       </c>
       <c r="L799" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M799" t="inlineStr"/>
@@ -35423,7 +35423,7 @@
       </c>
       <c r="L801" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M801" t="inlineStr"/>
@@ -35755,7 +35755,7 @@
       </c>
       <c r="L809" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M809" t="inlineStr"/>
@@ -35800,7 +35800,7 @@
       </c>
       <c r="L810" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M810" t="inlineStr"/>
@@ -36050,7 +36050,7 @@
       </c>
       <c r="L816" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M816" t="inlineStr"/>
@@ -36095,7 +36095,7 @@
       </c>
       <c r="L817" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M817" t="inlineStr"/>
@@ -36140,7 +36140,7 @@
       </c>
       <c r="L818" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M818" t="inlineStr"/>
@@ -36185,7 +36185,7 @@
       </c>
       <c r="L819" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M819" t="inlineStr"/>
@@ -36451,7 +36451,7 @@
       </c>
       <c r="L825" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
       <c r="M825" t="inlineStr"/>
@@ -36586,7 +36586,7 @@
       </c>
       <c r="L828" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M828" t="inlineStr"/>
@@ -36672,7 +36672,7 @@
       </c>
       <c r="L830" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M830" t="inlineStr"/>
@@ -36762,7 +36762,7 @@
       </c>
       <c r="L832" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M832" t="inlineStr"/>
@@ -37110,7 +37110,7 @@
       </c>
       <c r="L840" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M840" t="inlineStr"/>
@@ -37196,7 +37196,7 @@
       </c>
       <c r="L842" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M842" t="inlineStr"/>
@@ -37241,7 +37241,7 @@
       </c>
       <c r="L843" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M843" t="inlineStr"/>
@@ -37286,7 +37286,7 @@
       </c>
       <c r="L844" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M844" t="inlineStr"/>
@@ -37372,7 +37372,7 @@
       </c>
       <c r="L846" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M846" t="inlineStr"/>
@@ -37417,7 +37417,7 @@
       </c>
       <c r="L847" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M847" t="inlineStr"/>
@@ -37503,7 +37503,7 @@
       </c>
       <c r="L849" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M849" t="inlineStr"/>
@@ -37548,7 +37548,7 @@
       </c>
       <c r="L850" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M850" t="inlineStr"/>
@@ -37769,7 +37769,7 @@
       </c>
       <c r="L855" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M855" t="inlineStr"/>
@@ -38031,7 +38031,7 @@
       </c>
       <c r="L861" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M861" t="inlineStr"/>
@@ -38117,7 +38117,7 @@
       </c>
       <c r="L863" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M863" t="inlineStr"/>
@@ -38162,7 +38162,7 @@
       </c>
       <c r="L864" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M864" t="inlineStr"/>
@@ -38248,7 +38248,7 @@
       </c>
       <c r="L866" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M866" t="inlineStr"/>
@@ -38293,7 +38293,7 @@
       </c>
       <c r="L867" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M867" t="inlineStr"/>
@@ -38379,7 +38379,7 @@
       </c>
       <c r="L869" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M869" t="inlineStr"/>
@@ -38424,7 +38424,7 @@
       </c>
       <c r="L870" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M870" t="inlineStr"/>
@@ -38510,7 +38510,7 @@
       </c>
       <c r="L872" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M872" t="inlineStr"/>
@@ -38555,7 +38555,7 @@
       </c>
       <c r="L873" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M873" t="inlineStr"/>
@@ -38641,7 +38641,7 @@
       </c>
       <c r="L875" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M875" t="inlineStr"/>
@@ -38686,7 +38686,7 @@
       </c>
       <c r="L876" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M876" t="inlineStr"/>
@@ -38772,7 +38772,7 @@
       </c>
       <c r="L878" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M878" t="inlineStr"/>
@@ -38817,7 +38817,7 @@
       </c>
       <c r="L879" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M879" t="inlineStr"/>
@@ -38907,7 +38907,7 @@
       </c>
       <c r="L881" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M881" t="inlineStr"/>
@@ -38952,7 +38952,7 @@
       </c>
       <c r="L882" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M882" t="inlineStr"/>
@@ -39038,7 +39038,7 @@
       </c>
       <c r="L884" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M884" t="inlineStr"/>
@@ -39173,7 +39173,7 @@
       </c>
       <c r="L887" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M887" t="inlineStr"/>
@@ -39218,7 +39218,7 @@
       </c>
       <c r="L888" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M888" t="inlineStr"/>
@@ -39304,7 +39304,7 @@
       </c>
       <c r="L890" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M890" t="inlineStr"/>
@@ -39349,7 +39349,7 @@
       </c>
       <c r="L891" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M891" t="inlineStr"/>
@@ -39439,7 +39439,7 @@
       </c>
       <c r="L893" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M893" t="inlineStr"/>
@@ -39648,7 +39648,7 @@
       </c>
       <c r="L898" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M898" t="inlineStr"/>
@@ -39738,7 +39738,7 @@
       </c>
       <c r="L900" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M900" t="inlineStr"/>
@@ -39783,7 +39783,7 @@
       </c>
       <c r="L901" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M901" t="inlineStr"/>
@@ -39869,7 +39869,7 @@
       </c>
       <c r="L903" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M903" t="inlineStr"/>
@@ -40303,7 +40303,7 @@
       </c>
       <c r="L913" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M913" t="inlineStr"/>
@@ -40348,7 +40348,7 @@
       </c>
       <c r="L914" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M914" t="inlineStr"/>
@@ -40393,7 +40393,7 @@
       </c>
       <c r="L915" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M915" t="inlineStr"/>
@@ -40438,7 +40438,7 @@
       </c>
       <c r="L916" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M916" t="inlineStr"/>
@@ -40573,7 +40573,7 @@
       </c>
       <c r="L919" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M919" t="inlineStr"/>
@@ -40659,7 +40659,7 @@
       </c>
       <c r="L921" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M921" t="inlineStr"/>
@@ -40794,7 +40794,7 @@
       </c>
       <c r="L924" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M924" t="inlineStr"/>
@@ -40884,7 +40884,7 @@
       </c>
       <c r="L926" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M926" t="inlineStr"/>
@@ -40974,7 +40974,7 @@
       </c>
       <c r="L928" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M928" t="inlineStr"/>
@@ -41060,7 +41060,7 @@
       </c>
       <c r="L930" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M930" t="inlineStr"/>
@@ -41146,7 +41146,7 @@
       </c>
       <c r="L932" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M932" t="inlineStr"/>
@@ -41281,7 +41281,7 @@
       </c>
       <c r="L935" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M935" t="inlineStr"/>
@@ -41367,7 +41367,7 @@
       </c>
       <c r="L937" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M937" t="inlineStr"/>
@@ -41502,7 +41502,7 @@
       </c>
       <c r="L940" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M940" t="inlineStr"/>
@@ -41629,7 +41629,7 @@
       </c>
       <c r="L943" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M943" t="inlineStr"/>
@@ -41715,7 +41715,7 @@
       </c>
       <c r="L945" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M945" t="inlineStr"/>
@@ -41760,7 +41760,7 @@
       </c>
       <c r="L946" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M946" t="inlineStr"/>
@@ -41846,7 +41846,7 @@
       </c>
       <c r="L948" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M948" t="inlineStr"/>
@@ -41891,7 +41891,7 @@
       </c>
       <c r="L949" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M949" t="inlineStr"/>
@@ -41977,7 +41977,7 @@
       </c>
       <c r="L951" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M951" t="inlineStr"/>
@@ -42022,7 +42022,7 @@
       </c>
       <c r="L952" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M952" t="inlineStr"/>
@@ -42067,7 +42067,7 @@
       </c>
       <c r="L953" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M953" t="inlineStr"/>
@@ -42112,7 +42112,7 @@
       </c>
       <c r="L954" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M954" t="inlineStr"/>
@@ -42157,7 +42157,7 @@
       </c>
       <c r="L955" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M955" t="inlineStr"/>
@@ -42202,7 +42202,7 @@
       </c>
       <c r="L956" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M956" t="inlineStr"/>
@@ -42411,7 +42411,7 @@
       </c>
       <c r="L961" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M961" t="inlineStr"/>
@@ -42501,7 +42501,7 @@
       </c>
       <c r="L963" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M963" t="inlineStr"/>
@@ -42628,7 +42628,7 @@
       </c>
       <c r="L966" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M966" t="inlineStr"/>
@@ -42673,7 +42673,7 @@
       </c>
       <c r="L967" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M967" t="inlineStr"/>
@@ -42718,7 +42718,7 @@
       </c>
       <c r="L968" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M968" t="inlineStr"/>
@@ -42894,7 +42894,7 @@
       </c>
       <c r="L972" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M972" t="inlineStr"/>
@@ -42939,7 +42939,7 @@
       </c>
       <c r="L973" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M973" t="inlineStr"/>
@@ -43025,7 +43025,7 @@
       </c>
       <c r="L975" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M975" t="inlineStr"/>
@@ -43070,7 +43070,7 @@
       </c>
       <c r="L976" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M976" t="inlineStr"/>
@@ -43156,7 +43156,7 @@
       </c>
       <c r="L978" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M978" t="inlineStr"/>
@@ -43246,7 +43246,7 @@
       </c>
       <c r="L980" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M980" t="inlineStr"/>
@@ -43291,7 +43291,7 @@
       </c>
       <c r="L981" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M981" t="inlineStr"/>
@@ -43377,7 +43377,7 @@
       </c>
       <c r="L983" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M983" t="inlineStr"/>
@@ -43422,7 +43422,7 @@
       </c>
       <c r="L984" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M984" t="inlineStr"/>
@@ -43508,7 +43508,7 @@
       </c>
       <c r="L986" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M986" t="inlineStr"/>
@@ -43553,7 +43553,7 @@
       </c>
       <c r="L987" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M987" t="inlineStr"/>
@@ -43639,7 +43639,7 @@
       </c>
       <c r="L989" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M989" t="inlineStr"/>
@@ -43684,7 +43684,7 @@
       </c>
       <c r="L990" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M990" t="inlineStr"/>
@@ -43770,7 +43770,7 @@
       </c>
       <c r="L992" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M992" t="inlineStr"/>
@@ -43815,7 +43815,7 @@
       </c>
       <c r="L993" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M993" t="inlineStr"/>
@@ -43901,7 +43901,7 @@
       </c>
       <c r="L995" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M995" t="inlineStr"/>
@@ -43991,7 +43991,7 @@
       </c>
       <c r="L997" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M997" t="inlineStr"/>
@@ -44036,7 +44036,7 @@
       </c>
       <c r="L998" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M998" t="inlineStr"/>
@@ -44081,7 +44081,7 @@
       </c>
       <c r="L999" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M999" t="inlineStr"/>
@@ -44167,7 +44167,7 @@
       </c>
       <c r="L1001" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1001" t="inlineStr"/>
@@ -44212,7 +44212,7 @@
       </c>
       <c r="L1002" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1002" t="inlineStr"/>
@@ -44298,7 +44298,7 @@
       </c>
       <c r="L1004" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
       <c r="M1004" t="inlineStr"/>
@@ -44343,7 +44343,7 @@
       </c>
       <c r="L1005" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1005" t="inlineStr"/>
@@ -44388,7 +44388,7 @@
       </c>
       <c r="L1006" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1006" t="inlineStr"/>
@@ -44474,7 +44474,7 @@
       </c>
       <c r="L1008" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1008" t="inlineStr"/>
@@ -44519,7 +44519,7 @@
       </c>
       <c r="L1009" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1009" t="inlineStr"/>
@@ -44605,7 +44605,7 @@
       </c>
       <c r="L1011" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1011" t="inlineStr"/>
@@ -44695,7 +44695,7 @@
       </c>
       <c r="L1013" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1013" t="inlineStr"/>
@@ -44785,7 +44785,7 @@
       </c>
       <c r="L1015" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1015" t="inlineStr"/>
@@ -44912,7 +44912,7 @@
       </c>
       <c r="L1018" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1018" t="inlineStr"/>
@@ -44998,7 +44998,7 @@
       </c>
       <c r="L1020" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1020" t="inlineStr"/>
@@ -45125,7 +45125,7 @@
       </c>
       <c r="L1023" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1023" t="inlineStr"/>
@@ -45211,7 +45211,7 @@
       </c>
       <c r="L1025" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1025" t="inlineStr"/>
@@ -45256,7 +45256,7 @@
       </c>
       <c r="L1026" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1026" t="inlineStr"/>
@@ -45301,7 +45301,7 @@
       </c>
       <c r="L1027" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1027" t="inlineStr"/>
@@ -45391,7 +45391,7 @@
       </c>
       <c r="L1029" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1029" t="inlineStr"/>
@@ -45567,7 +45567,7 @@
       </c>
       <c r="L1033" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1033" t="inlineStr"/>
@@ -45657,7 +45657,7 @@
       </c>
       <c r="L1035" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1035" t="inlineStr"/>
@@ -45792,7 +45792,7 @@
       </c>
       <c r="L1038" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1038" t="inlineStr"/>
@@ -45837,7 +45837,7 @@
       </c>
       <c r="L1039" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1039" t="inlineStr"/>
@@ -45927,7 +45927,7 @@
       </c>
       <c r="L1041" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1041" t="inlineStr"/>
@@ -45972,7 +45972,7 @@
       </c>
       <c r="L1042" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1042" t="inlineStr"/>
@@ -46017,7 +46017,7 @@
       </c>
       <c r="L1043" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M1043" t="inlineStr"/>
@@ -46062,7 +46062,7 @@
       </c>
       <c r="L1044" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1044" t="inlineStr"/>
@@ -46107,7 +46107,7 @@
       </c>
       <c r="L1045" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1045" t="inlineStr"/>
@@ -46197,7 +46197,7 @@
       </c>
       <c r="L1047" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1047" t="inlineStr"/>
@@ -46242,7 +46242,7 @@
       </c>
       <c r="L1048" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1048" t="inlineStr"/>
@@ -46377,7 +46377,7 @@
       </c>
       <c r="L1051" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1051" t="inlineStr"/>
@@ -46639,7 +46639,7 @@
       </c>
       <c r="L1057" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1057" t="inlineStr"/>
@@ -46684,7 +46684,7 @@
       </c>
       <c r="L1058" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1058" t="inlineStr"/>
@@ -46819,7 +46819,7 @@
       </c>
       <c r="L1061" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1061" t="inlineStr"/>
@@ -46950,7 +46950,7 @@
       </c>
       <c r="L1064" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1064" t="inlineStr"/>
@@ -47085,7 +47085,7 @@
       </c>
       <c r="L1067" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1067" t="inlineStr"/>
@@ -47827,7 +47827,7 @@
       </c>
       <c r="L1085" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1085" t="inlineStr"/>
@@ -47917,7 +47917,7 @@
       </c>
       <c r="L1087" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1087" t="inlineStr"/>
@@ -48044,7 +48044,7 @@
       </c>
       <c r="L1090" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M1090" t="inlineStr"/>
@@ -48089,7 +48089,7 @@
       </c>
       <c r="L1091" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1091" t="inlineStr"/>
@@ -48175,7 +48175,7 @@
       </c>
       <c r="L1093" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1093" t="inlineStr"/>
@@ -48261,7 +48261,7 @@
       </c>
       <c r="L1095" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1095" t="inlineStr"/>
@@ -48351,7 +48351,7 @@
       </c>
       <c r="L1097" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1097" t="inlineStr"/>
@@ -48396,7 +48396,7 @@
       </c>
       <c r="L1098" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1098" t="inlineStr"/>
@@ -48929,7 +48929,7 @@
       </c>
       <c r="L1111" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1111" t="inlineStr"/>
@@ -49019,7 +49019,7 @@
       </c>
       <c r="L1113" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1113" t="inlineStr"/>
@@ -49064,7 +49064,7 @@
       </c>
       <c r="L1114" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1114" t="inlineStr"/>
@@ -49154,7 +49154,7 @@
       </c>
       <c r="L1116" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1116" t="inlineStr"/>
@@ -49461,7 +49461,7 @@
       </c>
       <c r="L1123" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1123" t="inlineStr"/>
@@ -49547,7 +49547,7 @@
       </c>
       <c r="L1125" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1125" t="inlineStr"/>
@@ -49637,7 +49637,7 @@
       </c>
       <c r="L1127" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1127" t="inlineStr"/>
@@ -49805,7 +49805,7 @@
       </c>
       <c r="L1131" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1131" t="inlineStr"/>
@@ -49891,7 +49891,7 @@
       </c>
       <c r="L1133" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1133" t="inlineStr"/>
@@ -50018,7 +50018,7 @@
       </c>
       <c r="L1136" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1136" t="inlineStr"/>
@@ -50108,7 +50108,7 @@
       </c>
       <c r="L1138" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1138" t="inlineStr"/>
@@ -50153,7 +50153,7 @@
       </c>
       <c r="L1139" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1139" t="inlineStr"/>
@@ -50243,7 +50243,7 @@
       </c>
       <c r="L1141" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1141" t="inlineStr"/>
@@ -50288,7 +50288,7 @@
       </c>
       <c r="L1142" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1142" t="inlineStr"/>
@@ -50333,7 +50333,7 @@
       </c>
       <c r="L1143" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1143" t="inlineStr"/>
@@ -50378,7 +50378,7 @@
       </c>
       <c r="L1144" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1144" t="inlineStr"/>
@@ -50423,7 +50423,7 @@
       </c>
       <c r="L1145" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1145" t="inlineStr"/>
@@ -50718,7 +50718,7 @@
       </c>
       <c r="L1152" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1152" t="inlineStr"/>
@@ -50976,7 +50976,7 @@
       </c>
       <c r="L1158" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1158" t="inlineStr"/>
@@ -51062,7 +51062,7 @@
       </c>
       <c r="L1160" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1160" t="inlineStr"/>
@@ -51107,7 +51107,7 @@
       </c>
       <c r="L1161" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1161" t="inlineStr"/>
@@ -51193,7 +51193,7 @@
       </c>
       <c r="L1163" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1163" t="inlineStr"/>
@@ -51238,7 +51238,7 @@
       </c>
       <c r="L1164" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M1164" t="inlineStr"/>
@@ -51328,7 +51328,7 @@
       </c>
       <c r="L1166" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1166" t="inlineStr"/>
@@ -51373,7 +51373,7 @@
       </c>
       <c r="L1167" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1167" t="inlineStr"/>
@@ -51459,7 +51459,7 @@
       </c>
       <c r="L1169" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1169" t="inlineStr"/>
@@ -51504,7 +51504,7 @@
       </c>
       <c r="L1170" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1170" t="inlineStr"/>
@@ -51590,7 +51590,7 @@
       </c>
       <c r="L1172" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1172" t="inlineStr"/>
@@ -51635,7 +51635,7 @@
       </c>
       <c r="L1173" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M1173" t="inlineStr"/>
@@ -51680,7 +51680,7 @@
       </c>
       <c r="L1174" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1174" t="inlineStr"/>
@@ -51725,7 +51725,7 @@
       </c>
       <c r="L1175" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1175" t="inlineStr"/>
@@ -51811,7 +51811,7 @@
       </c>
       <c r="L1177" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1177" t="inlineStr"/>
@@ -51901,7 +51901,7 @@
       </c>
       <c r="L1179" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1179" t="inlineStr"/>
@@ -52352,7 +52352,7 @@
       </c>
       <c r="L1190" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1190" t="inlineStr"/>
@@ -52442,7 +52442,7 @@
       </c>
       <c r="L1192" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1192" t="inlineStr"/>
@@ -52614,7 +52614,7 @@
       </c>
       <c r="L1196" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1196" t="inlineStr"/>
@@ -52704,7 +52704,7 @@
       </c>
       <c r="L1198" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1198" t="inlineStr"/>
@@ -52749,7 +52749,7 @@
       </c>
       <c r="L1199" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1199" t="inlineStr"/>
@@ -52839,7 +52839,7 @@
       </c>
       <c r="L1201" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1201" t="inlineStr"/>
@@ -52884,7 +52884,7 @@
       </c>
       <c r="L1202" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1202" t="inlineStr"/>
@@ -52970,7 +52970,7 @@
       </c>
       <c r="L1204" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
       <c r="M1204" t="inlineStr"/>
@@ -53015,7 +53015,7 @@
       </c>
       <c r="L1205" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1205" t="inlineStr"/>
@@ -53236,7 +53236,7 @@
       </c>
       <c r="L1210" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1210" t="inlineStr"/>
@@ -53322,7 +53322,7 @@
       </c>
       <c r="L1212" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
       <c r="M1212" t="inlineStr"/>
@@ -53367,7 +53367,7 @@
       </c>
       <c r="L1213" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1213" t="inlineStr"/>
@@ -53457,7 +53457,7 @@
       </c>
       <c r="L1215" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M1215" t="inlineStr"/>
@@ -53502,7 +53502,7 @@
       </c>
       <c r="L1216" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1216" t="inlineStr"/>
@@ -53629,7 +53629,7 @@
       </c>
       <c r="L1219" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1219" t="inlineStr"/>
@@ -53674,7 +53674,7 @@
       </c>
       <c r="L1220" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1220" t="inlineStr"/>
@@ -53719,7 +53719,7 @@
       </c>
       <c r="L1221" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1221" t="inlineStr"/>
@@ -53764,7 +53764,7 @@
       </c>
       <c r="L1222" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1222" t="inlineStr"/>
@@ -53809,7 +53809,7 @@
       </c>
       <c r="L1223" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1223" t="inlineStr"/>
@@ -53940,7 +53940,7 @@
       </c>
       <c r="L1226" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1226" t="inlineStr"/>
@@ -54030,7 +54030,7 @@
       </c>
       <c r="L1228" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1228" t="inlineStr"/>
@@ -54366,7 +54366,7 @@
       </c>
       <c r="L1236" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1236" t="inlineStr"/>
@@ -54411,7 +54411,7 @@
       </c>
       <c r="L1237" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1237" t="inlineStr"/>
@@ -54501,7 +54501,7 @@
       </c>
       <c r="L1239" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1239" t="inlineStr"/>
@@ -54636,7 +54636,7 @@
       </c>
       <c r="L1242" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1242" t="inlineStr"/>
@@ -54722,7 +54722,7 @@
       </c>
       <c r="L1244" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1244" t="inlineStr"/>
@@ -54767,7 +54767,7 @@
       </c>
       <c r="L1245" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1245" t="inlineStr"/>
@@ -54853,7 +54853,7 @@
       </c>
       <c r="L1247" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1247" t="inlineStr"/>
@@ -54898,7 +54898,7 @@
       </c>
       <c r="L1248" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1248" t="inlineStr"/>
@@ -54984,7 +54984,7 @@
       </c>
       <c r="L1250" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1250" t="inlineStr"/>
@@ -55029,7 +55029,7 @@
       </c>
       <c r="L1251" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1251" t="inlineStr"/>
@@ -55115,7 +55115,7 @@
       </c>
       <c r="L1253" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1253" t="inlineStr"/>
@@ -55160,7 +55160,7 @@
       </c>
       <c r="L1254" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1254" t="inlineStr"/>
@@ -55246,7 +55246,7 @@
       </c>
       <c r="L1256" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1256" t="inlineStr"/>
@@ -55291,7 +55291,7 @@
       </c>
       <c r="L1257" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1257" t="inlineStr"/>
@@ -55377,7 +55377,7 @@
       </c>
       <c r="L1259" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1259" t="inlineStr"/>
@@ -55422,7 +55422,7 @@
       </c>
       <c r="L1260" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1260" t="inlineStr"/>
@@ -55508,7 +55508,7 @@
       </c>
       <c r="L1262" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1262" t="inlineStr"/>
@@ -55553,7 +55553,7 @@
       </c>
       <c r="L1263" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1263" t="inlineStr"/>
@@ -55598,7 +55598,7 @@
       </c>
       <c r="L1264" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M1264" t="inlineStr"/>
@@ -55643,7 +55643,7 @@
       </c>
       <c r="L1265" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1265" t="inlineStr"/>
@@ -55688,7 +55688,7 @@
       </c>
       <c r="L1266" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1266" t="inlineStr"/>
@@ -55774,7 +55774,7 @@
       </c>
       <c r="L1268" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1268" t="inlineStr"/>
@@ -55819,7 +55819,7 @@
       </c>
       <c r="L1269" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1269" t="inlineStr"/>
@@ -55905,7 +55905,7 @@
       </c>
       <c r="L1271" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1271" t="inlineStr"/>
@@ -55995,7 +55995,7 @@
       </c>
       <c r="L1273" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1273" t="inlineStr"/>
@@ -56040,7 +56040,7 @@
       </c>
       <c r="L1274" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1274" t="inlineStr"/>
@@ -56126,7 +56126,7 @@
       </c>
       <c r="L1276" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1276" t="inlineStr"/>
@@ -56384,7 +56384,7 @@
       </c>
       <c r="L1282" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1282" t="inlineStr"/>
@@ -56429,7 +56429,7 @@
       </c>
       <c r="L1283" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1283" t="inlineStr"/>
@@ -56515,7 +56515,7 @@
       </c>
       <c r="L1285" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1285" t="inlineStr"/>
@@ -56605,7 +56605,7 @@
       </c>
       <c r="L1287" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1287" t="inlineStr"/>
@@ -56945,7 +56945,7 @@
       </c>
       <c r="L1295" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M1295" t="inlineStr"/>
@@ -56990,7 +56990,7 @@
       </c>
       <c r="L1296" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1296" t="inlineStr"/>
@@ -57121,7 +57121,7 @@
       </c>
       <c r="L1299" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1299" t="inlineStr"/>
@@ -57412,7 +57412,7 @@
       </c>
       <c r="L1306" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1306" t="inlineStr"/>
@@ -57502,7 +57502,7 @@
       </c>
       <c r="L1308" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1308" t="inlineStr"/>
@@ -57588,7 +57588,7 @@
       </c>
       <c r="L1310" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1310" t="inlineStr"/>
@@ -57838,7 +57838,7 @@
       </c>
       <c r="L1316" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1316" t="inlineStr"/>
@@ -57924,7 +57924,7 @@
       </c>
       <c r="L1318" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1318" t="inlineStr"/>
@@ -58014,7 +58014,7 @@
       </c>
       <c r="L1320" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1320" t="inlineStr"/>
@@ -58059,7 +58059,7 @@
       </c>
       <c r="L1321" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1321" t="inlineStr"/>
@@ -58149,7 +58149,7 @@
       </c>
       <c r="L1323" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1323" t="inlineStr"/>
@@ -58194,7 +58194,7 @@
       </c>
       <c r="L1324" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M1324" t="inlineStr"/>
@@ -58239,7 +58239,7 @@
       </c>
       <c r="L1325" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1325" t="inlineStr"/>
@@ -58325,7 +58325,7 @@
       </c>
       <c r="L1327" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1327" t="inlineStr"/>
@@ -58411,7 +58411,7 @@
       </c>
       <c r="L1329" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1329" t="inlineStr"/>
@@ -58497,7 +58497,7 @@
       </c>
       <c r="L1331" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1331" t="inlineStr"/>
@@ -58583,7 +58583,7 @@
       </c>
       <c r="L1333" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1333" t="inlineStr"/>
@@ -58669,7 +58669,7 @@
       </c>
       <c r="L1335" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1335" t="inlineStr"/>
@@ -58759,7 +58759,7 @@
       </c>
       <c r="L1337" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1337" t="inlineStr"/>
@@ -58849,7 +58849,7 @@
       </c>
       <c r="L1339" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1339" t="inlineStr"/>
@@ -58894,7 +58894,7 @@
       </c>
       <c r="L1340" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1340" t="inlineStr"/>
@@ -58980,7 +58980,7 @@
       </c>
       <c r="L1342" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1342" t="inlineStr"/>
@@ -59115,7 +59115,7 @@
       </c>
       <c r="L1345" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1345" t="inlineStr"/>
@@ -59250,7 +59250,7 @@
       </c>
       <c r="L1348" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1348" t="inlineStr"/>
@@ -59295,7 +59295,7 @@
       </c>
       <c r="L1349" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M1349" t="inlineStr"/>
@@ -59340,7 +59340,7 @@
       </c>
       <c r="L1350" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1350" t="inlineStr"/>
@@ -59512,7 +59512,7 @@
       </c>
       <c r="L1354" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1354" t="inlineStr"/>
@@ -59598,7 +59598,7 @@
       </c>
       <c r="L1356" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1356" t="inlineStr"/>
@@ -59643,7 +59643,7 @@
       </c>
       <c r="L1357" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1357" t="inlineStr"/>
@@ -59729,7 +59729,7 @@
       </c>
       <c r="L1359" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
       <c r="M1359" t="inlineStr"/>
@@ -59774,7 +59774,7 @@
       </c>
       <c r="L1360" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1360" t="inlineStr"/>
@@ -59819,7 +59819,7 @@
       </c>
       <c r="L1361" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1361" t="inlineStr"/>
@@ -59905,7 +59905,7 @@
       </c>
       <c r="L1363" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1363" t="inlineStr"/>
@@ -59950,7 +59950,7 @@
       </c>
       <c r="L1364" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1364" t="inlineStr"/>
@@ -60036,7 +60036,7 @@
       </c>
       <c r="L1366" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1366" t="inlineStr"/>
@@ -60126,7 +60126,7 @@
       </c>
       <c r="L1368" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1368" t="inlineStr"/>
@@ -60212,7 +60212,7 @@
       </c>
       <c r="L1370" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1370" t="inlineStr"/>
@@ -60302,7 +60302,7 @@
       </c>
       <c r="L1372" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1372" t="inlineStr"/>
@@ -60478,7 +60478,7 @@
       </c>
       <c r="L1376" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1376" t="inlineStr"/>
@@ -60523,7 +60523,7 @@
       </c>
       <c r="L1377" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M1377" t="inlineStr"/>
@@ -60568,7 +60568,7 @@
       </c>
       <c r="L1378" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1378" t="inlineStr"/>
@@ -60613,7 +60613,7 @@
       </c>
       <c r="L1379" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1379" t="inlineStr"/>
@@ -60744,7 +60744,7 @@
       </c>
       <c r="L1382" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1382" t="inlineStr"/>
@@ -60830,7 +60830,7 @@
       </c>
       <c r="L1384" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1384" t="inlineStr"/>
@@ -60965,7 +60965,7 @@
       </c>
       <c r="L1387" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1387" t="inlineStr"/>
@@ -61010,7 +61010,7 @@
       </c>
       <c r="L1388" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1388" t="inlineStr"/>
@@ -61096,7 +61096,7 @@
       </c>
       <c r="L1390" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1390" t="inlineStr"/>
@@ -61186,7 +61186,7 @@
       </c>
       <c r="L1392" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1392" t="inlineStr"/>
@@ -61407,7 +61407,7 @@
       </c>
       <c r="L1397" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1397" t="inlineStr"/>
@@ -61452,7 +61452,7 @@
       </c>
       <c r="L1398" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M1398" t="inlineStr"/>
@@ -61497,7 +61497,7 @@
       </c>
       <c r="L1399" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1399" t="inlineStr"/>
@@ -61542,7 +61542,7 @@
       </c>
       <c r="L1400" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1400" t="inlineStr"/>
@@ -61632,7 +61632,7 @@
       </c>
       <c r="L1402" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1402" t="inlineStr"/>
@@ -61804,7 +61804,7 @@
       </c>
       <c r="L1406" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M1406" t="inlineStr"/>
@@ -61849,7 +61849,7 @@
       </c>
       <c r="L1407" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1407" t="inlineStr"/>
@@ -61894,7 +61894,7 @@
       </c>
       <c r="L1408" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1408" t="inlineStr"/>
@@ -61980,7 +61980,7 @@
       </c>
       <c r="L1410" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1410" t="inlineStr"/>
@@ -62111,7 +62111,7 @@
       </c>
       <c r="L1413" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
       <c r="M1413" t="inlineStr"/>
@@ -62156,7 +62156,7 @@
       </c>
       <c r="L1414" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
       <c r="M1414" t="inlineStr"/>

</xml_diff>

<commit_message>
run script again, compile new attributions
</commit_message>
<xml_diff>
--- a/WD_BDRC_data.xlsx
+++ b/WD_BDRC_data.xlsx
@@ -593,7 +593,7 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
@@ -716,7 +716,7 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
@@ -847,7 +847,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
@@ -892,7 +892,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M10" t="inlineStr"/>
@@ -982,7 +982,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M12" t="inlineStr"/>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M13" t="inlineStr"/>
@@ -1072,7 +1072,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M14" t="inlineStr"/>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M15" t="inlineStr"/>
@@ -1162,7 +1162,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M16" t="inlineStr"/>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M19" t="inlineStr"/>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M20" t="inlineStr"/>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M22" t="inlineStr"/>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M23" t="inlineStr"/>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M25" t="inlineStr"/>
@@ -1612,7 +1612,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M26" t="inlineStr"/>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M28" t="inlineStr"/>
@@ -1792,7 +1792,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M30" t="inlineStr"/>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="M31" t="inlineStr"/>
@@ -1968,7 +1968,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="M34" t="inlineStr"/>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="M37" t="inlineStr"/>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M40" t="inlineStr"/>
@@ -2316,7 +2316,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M42" t="inlineStr"/>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M43" t="inlineStr"/>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M44" t="inlineStr"/>
@@ -2451,7 +2451,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M45" t="inlineStr"/>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M47" t="inlineStr"/>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M48" t="inlineStr"/>
@@ -2676,7 +2676,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M50" t="inlineStr"/>
@@ -2721,7 +2721,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M51" t="inlineStr"/>
@@ -2811,7 +2811,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M53" t="inlineStr"/>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M54" t="inlineStr"/>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M56" t="inlineStr"/>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M59" t="inlineStr"/>
@@ -3204,7 +3204,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="M62" t="inlineStr"/>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M63" t="inlineStr"/>
@@ -3339,7 +3339,7 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M65" t="inlineStr"/>
@@ -3429,7 +3429,7 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M67" t="inlineStr"/>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M69" t="inlineStr"/>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M71" t="inlineStr"/>
@@ -3654,7 +3654,7 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M72" t="inlineStr"/>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M73" t="inlineStr"/>
@@ -3744,7 +3744,7 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M74" t="inlineStr"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M75" t="inlineStr"/>
@@ -3834,7 +3834,7 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M76" t="inlineStr"/>
@@ -3879,7 +3879,7 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M77" t="inlineStr"/>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M79" t="inlineStr"/>
@@ -4014,7 +4014,7 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M80" t="inlineStr"/>
@@ -4149,7 +4149,7 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M83" t="inlineStr"/>
@@ -4194,7 +4194,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M84" t="inlineStr"/>
@@ -4284,7 +4284,7 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M86" t="inlineStr"/>
@@ -4419,7 +4419,7 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M89" t="inlineStr"/>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M91" t="inlineStr"/>
@@ -4550,7 +4550,7 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M92" t="inlineStr"/>
@@ -4636,7 +4636,7 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M94" t="inlineStr"/>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M97" t="inlineStr"/>
@@ -4906,7 +4906,7 @@
       </c>
       <c r="L100" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
       <c r="M100" t="inlineStr"/>
@@ -5246,7 +5246,7 @@
       </c>
       <c r="L108" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M108" t="inlineStr"/>
@@ -5291,7 +5291,7 @@
       </c>
       <c r="L109" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="M109" t="inlineStr"/>
@@ -5471,7 +5471,7 @@
       </c>
       <c r="L113" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M113" t="inlineStr"/>
@@ -5606,7 +5606,7 @@
       </c>
       <c r="L116" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M116" t="inlineStr"/>
@@ -5696,7 +5696,7 @@
       </c>
       <c r="L118" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
       <c r="M118" t="inlineStr"/>
@@ -5782,7 +5782,7 @@
       </c>
       <c r="L120" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M120" t="inlineStr"/>
@@ -5827,7 +5827,7 @@
       </c>
       <c r="L121" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M121" t="inlineStr"/>
@@ -5913,7 +5913,7 @@
       </c>
       <c r="L123" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M123" t="inlineStr"/>
@@ -6003,7 +6003,7 @@
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M125" t="inlineStr"/>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M127" t="inlineStr"/>
@@ -6138,7 +6138,7 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M128" t="inlineStr"/>
@@ -6269,7 +6269,7 @@
       </c>
       <c r="L131" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M131" t="inlineStr"/>
@@ -6539,7 +6539,7 @@
       </c>
       <c r="L137" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M137" t="inlineStr"/>
@@ -6584,7 +6584,7 @@
       </c>
       <c r="L138" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M138" t="inlineStr"/>
@@ -6674,7 +6674,7 @@
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M140" t="inlineStr"/>
@@ -6719,7 +6719,7 @@
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M141" t="inlineStr"/>
@@ -6809,7 +6809,7 @@
       </c>
       <c r="L143" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M143" t="inlineStr"/>
@@ -6899,7 +6899,7 @@
       </c>
       <c r="L145" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M145" t="inlineStr"/>
@@ -6944,7 +6944,7 @@
       </c>
       <c r="L146" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M146" t="inlineStr"/>
@@ -6989,7 +6989,7 @@
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M147" t="inlineStr"/>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="L149" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M149" t="inlineStr"/>
@@ -7120,7 +7120,7 @@
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M150" t="inlineStr"/>
@@ -7210,7 +7210,7 @@
       </c>
       <c r="L152" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M152" t="inlineStr"/>
@@ -7300,7 +7300,7 @@
       </c>
       <c r="L154" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M154" t="inlineStr"/>
@@ -7390,7 +7390,7 @@
       </c>
       <c r="L156" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M156" t="inlineStr"/>
@@ -7525,7 +7525,7 @@
       </c>
       <c r="L159" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M159" t="inlineStr"/>
@@ -7570,7 +7570,7 @@
       </c>
       <c r="L160" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M160" t="inlineStr"/>
@@ -7701,7 +7701,7 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M163" t="inlineStr"/>
@@ -7746,7 +7746,7 @@
       </c>
       <c r="L164" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M164" t="inlineStr"/>
@@ -7877,7 +7877,7 @@
       </c>
       <c r="L167" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M167" t="inlineStr"/>
@@ -7922,7 +7922,7 @@
       </c>
       <c r="L168" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M168" t="inlineStr"/>
@@ -8012,7 +8012,7 @@
       </c>
       <c r="L170" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M170" t="inlineStr"/>
@@ -8057,7 +8057,7 @@
       </c>
       <c r="L171" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M171" t="inlineStr"/>
@@ -8188,7 +8188,7 @@
       </c>
       <c r="L174" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M174" t="inlineStr"/>
@@ -8278,7 +8278,7 @@
       </c>
       <c r="L176" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M176" t="inlineStr"/>
@@ -8323,7 +8323,7 @@
       </c>
       <c r="L177" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M177" t="inlineStr"/>
@@ -8413,7 +8413,7 @@
       </c>
       <c r="L179" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
       <c r="M179" t="inlineStr"/>
@@ -8458,7 +8458,7 @@
       </c>
       <c r="L180" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M180" t="inlineStr"/>
@@ -8503,7 +8503,7 @@
       </c>
       <c r="L181" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M181" t="inlineStr"/>
@@ -8548,7 +8548,7 @@
       </c>
       <c r="L182" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M182" t="inlineStr"/>
@@ -8683,7 +8683,7 @@
       </c>
       <c r="L185" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M185" t="inlineStr"/>
@@ -8818,7 +8818,7 @@
       </c>
       <c r="L188" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M188" t="inlineStr"/>
@@ -8863,7 +8863,7 @@
       </c>
       <c r="L189" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
       <c r="M189" t="inlineStr"/>
@@ -8953,7 +8953,7 @@
       </c>
       <c r="L191" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M191" t="inlineStr"/>
@@ -9088,7 +9088,7 @@
       </c>
       <c r="L194" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M194" t="inlineStr"/>
@@ -9133,7 +9133,7 @@
       </c>
       <c r="L195" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="M195" t="inlineStr"/>
@@ -9178,7 +9178,7 @@
       </c>
       <c r="L196" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="M196" t="inlineStr"/>
@@ -9223,7 +9223,7 @@
       </c>
       <c r="L197" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M197" t="inlineStr"/>
@@ -9448,7 +9448,7 @@
       </c>
       <c r="L202" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M202" t="inlineStr"/>
@@ -9493,7 +9493,7 @@
       </c>
       <c r="L203" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M203" t="inlineStr"/>
@@ -9538,7 +9538,7 @@
       </c>
       <c r="L204" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M204" t="inlineStr"/>
@@ -9628,7 +9628,7 @@
       </c>
       <c r="L206" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M206" t="inlineStr"/>
@@ -9673,7 +9673,7 @@
       </c>
       <c r="L207" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M207" t="inlineStr"/>
@@ -9759,7 +9759,7 @@
       </c>
       <c r="L209" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M209" t="inlineStr"/>
@@ -9894,7 +9894,7 @@
       </c>
       <c r="L212" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M212" t="inlineStr"/>
@@ -9939,7 +9939,7 @@
       </c>
       <c r="L213" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M213" t="inlineStr"/>
@@ -10025,7 +10025,7 @@
       </c>
       <c r="L215" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M215" t="inlineStr"/>
@@ -10160,7 +10160,7 @@
       </c>
       <c r="L218" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
       <c r="M218" t="inlineStr"/>
@@ -10205,7 +10205,7 @@
       </c>
       <c r="L219" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
       <c r="M219" t="inlineStr"/>
@@ -10295,7 +10295,7 @@
       </c>
       <c r="L221" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M221" t="inlineStr"/>
@@ -10340,7 +10340,7 @@
       </c>
       <c r="L222" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M222" t="inlineStr"/>
@@ -10430,7 +10430,7 @@
       </c>
       <c r="L224" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M224" t="inlineStr"/>
@@ -10520,7 +10520,7 @@
       </c>
       <c r="L226" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M226" t="inlineStr"/>
@@ -10565,7 +10565,7 @@
       </c>
       <c r="L227" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
       <c r="M227" t="inlineStr"/>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="L229" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M229" t="inlineStr"/>
@@ -10700,7 +10700,7 @@
       </c>
       <c r="L230" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M230" t="inlineStr"/>
@@ -10790,7 +10790,7 @@
       </c>
       <c r="L232" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M232" t="inlineStr"/>
@@ -10880,7 +10880,7 @@
       </c>
       <c r="L234" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M234" t="inlineStr"/>
@@ -10925,7 +10925,7 @@
       </c>
       <c r="L235" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M235" t="inlineStr"/>
@@ -11015,7 +11015,7 @@
       </c>
       <c r="L237" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M237" t="inlineStr"/>
@@ -11060,7 +11060,7 @@
       </c>
       <c r="L238" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="M238" t="inlineStr"/>
@@ -11105,7 +11105,7 @@
       </c>
       <c r="L239" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M239" t="inlineStr"/>
@@ -11236,7 +11236,7 @@
       </c>
       <c r="L242" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
       <c r="M242" t="inlineStr"/>
@@ -11506,7 +11506,7 @@
       </c>
       <c r="L248" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M248" t="inlineStr"/>
@@ -11551,7 +11551,7 @@
       </c>
       <c r="L249" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M249" t="inlineStr"/>
@@ -11596,7 +11596,7 @@
       </c>
       <c r="L250" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M250" t="inlineStr"/>
@@ -11682,7 +11682,7 @@
       </c>
       <c r="L252" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M252" t="inlineStr"/>
@@ -11772,7 +11772,7 @@
       </c>
       <c r="L254" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M254" t="inlineStr"/>
@@ -11862,7 +11862,7 @@
       </c>
       <c r="L256" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M256" t="inlineStr"/>
@@ -11952,7 +11952,7 @@
       </c>
       <c r="L258" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M258" t="inlineStr"/>
@@ -12042,7 +12042,7 @@
       </c>
       <c r="L260" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M260" t="inlineStr"/>
@@ -12169,7 +12169,7 @@
       </c>
       <c r="L263" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M263" t="inlineStr"/>
@@ -12214,7 +12214,7 @@
       </c>
       <c r="L264" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
       <c r="M264" t="inlineStr"/>
@@ -12259,7 +12259,7 @@
       </c>
       <c r="L265" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M265" t="inlineStr"/>
@@ -12345,7 +12345,7 @@
       </c>
       <c r="L267" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M267" t="inlineStr"/>
@@ -12435,7 +12435,7 @@
       </c>
       <c r="L269" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M269" t="inlineStr"/>
@@ -12570,7 +12570,7 @@
       </c>
       <c r="L272" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M272" t="inlineStr"/>
@@ -12750,7 +12750,7 @@
       </c>
       <c r="L276" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M276" t="inlineStr"/>
@@ -12795,7 +12795,7 @@
       </c>
       <c r="L277" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="M277" t="inlineStr"/>
@@ -13106,7 +13106,7 @@
       </c>
       <c r="L284" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="M284" t="inlineStr"/>
@@ -13401,7 +13401,7 @@
       </c>
       <c r="L291" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M291" t="inlineStr"/>
@@ -13491,7 +13491,7 @@
       </c>
       <c r="L293" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
       <c r="M293" t="inlineStr"/>
@@ -13618,7 +13618,7 @@
       </c>
       <c r="L296" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M296" t="inlineStr"/>
@@ -13704,7 +13704,7 @@
       </c>
       <c r="L298" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M298" t="inlineStr"/>
@@ -13749,7 +13749,7 @@
       </c>
       <c r="L299" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M299" t="inlineStr"/>
@@ -13835,7 +13835,7 @@
       </c>
       <c r="L301" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M301" t="inlineStr"/>
@@ -13880,7 +13880,7 @@
       </c>
       <c r="L302" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M302" t="inlineStr"/>
@@ -13970,7 +13970,7 @@
       </c>
       <c r="L304" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M304" t="inlineStr"/>
@@ -14015,7 +14015,7 @@
       </c>
       <c r="L305" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M305" t="inlineStr"/>
@@ -14101,7 +14101,7 @@
       </c>
       <c r="L307" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M307" t="inlineStr"/>
@@ -14187,7 +14187,7 @@
       </c>
       <c r="L309" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
       <c r="M309" t="inlineStr"/>
@@ -14273,7 +14273,7 @@
       </c>
       <c r="L311" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M311" t="inlineStr"/>
@@ -14363,7 +14363,7 @@
       </c>
       <c r="L313" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M313" t="inlineStr"/>
@@ -14453,7 +14453,7 @@
       </c>
       <c r="L315" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
       <c r="M315" t="inlineStr"/>
@@ -14498,7 +14498,7 @@
       </c>
       <c r="L316" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M316" t="inlineStr"/>
@@ -14588,7 +14588,7 @@
       </c>
       <c r="L318" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M318" t="inlineStr"/>
@@ -14723,7 +14723,7 @@
       </c>
       <c r="L321" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M321" t="inlineStr"/>
@@ -14813,7 +14813,7 @@
       </c>
       <c r="L323" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M323" t="inlineStr"/>
@@ -14858,7 +14858,7 @@
       </c>
       <c r="L324" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M324" t="inlineStr"/>
@@ -14944,7 +14944,7 @@
       </c>
       <c r="L326" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M326" t="inlineStr"/>
@@ -14989,7 +14989,7 @@
       </c>
       <c r="L327" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M327" t="inlineStr"/>
@@ -15079,7 +15079,7 @@
       </c>
       <c r="L329" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M329" t="inlineStr"/>
@@ -15169,7 +15169,7 @@
       </c>
       <c r="L331" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M331" t="inlineStr"/>
@@ -15214,7 +15214,7 @@
       </c>
       <c r="L332" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="M332" t="inlineStr"/>
@@ -15304,7 +15304,7 @@
       </c>
       <c r="L334" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M334" t="inlineStr"/>
@@ -15394,7 +15394,7 @@
       </c>
       <c r="L336" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M336" t="inlineStr"/>
@@ -15484,7 +15484,7 @@
       </c>
       <c r="L338" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
       <c r="M338" t="inlineStr"/>
@@ -15574,7 +15574,7 @@
       </c>
       <c r="L340" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M340" t="inlineStr"/>
@@ -15664,7 +15664,7 @@
       </c>
       <c r="L342" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M342" t="inlineStr"/>
@@ -15709,7 +15709,7 @@
       </c>
       <c r="L343" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M343" t="inlineStr"/>
@@ -15799,7 +15799,7 @@
       </c>
       <c r="L345" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M345" t="inlineStr"/>
@@ -15844,7 +15844,7 @@
       </c>
       <c r="L346" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M346" t="inlineStr"/>
@@ -15934,7 +15934,7 @@
       </c>
       <c r="L348" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M348" t="inlineStr"/>
@@ -16110,7 +16110,7 @@
       </c>
       <c r="L352" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M352" t="inlineStr"/>
@@ -16245,7 +16245,7 @@
       </c>
       <c r="L355" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M355" t="inlineStr"/>
@@ -16376,7 +16376,7 @@
       </c>
       <c r="L358" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M358" t="inlineStr"/>
@@ -16511,7 +16511,7 @@
       </c>
       <c r="L361" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M361" t="inlineStr"/>
@@ -16601,7 +16601,7 @@
       </c>
       <c r="L363" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M363" t="inlineStr"/>
@@ -16646,7 +16646,7 @@
       </c>
       <c r="L364" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M364" t="inlineStr"/>
@@ -16732,7 +16732,7 @@
       </c>
       <c r="L366" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M366" t="inlineStr"/>
@@ -16777,7 +16777,7 @@
       </c>
       <c r="L367" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M367" t="inlineStr"/>
@@ -16863,7 +16863,7 @@
       </c>
       <c r="L369" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M369" t="inlineStr"/>
@@ -16908,7 +16908,7 @@
       </c>
       <c r="L370" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M370" t="inlineStr"/>
@@ -17080,7 +17080,7 @@
       </c>
       <c r="L374" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M374" t="inlineStr"/>
@@ -17125,7 +17125,7 @@
       </c>
       <c r="L375" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M375" t="inlineStr"/>
@@ -17215,7 +17215,7 @@
       </c>
       <c r="L377" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M377" t="inlineStr"/>
@@ -17481,7 +17481,7 @@
       </c>
       <c r="L383" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M383" t="inlineStr"/>
@@ -17526,7 +17526,7 @@
       </c>
       <c r="L384" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M384" t="inlineStr"/>
@@ -17657,7 +17657,7 @@
       </c>
       <c r="L387" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M387" t="inlineStr"/>
@@ -17878,7 +17878,7 @@
       </c>
       <c r="L392" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
       <c r="M392" t="inlineStr"/>
@@ -17923,7 +17923,7 @@
       </c>
       <c r="L393" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M393" t="inlineStr"/>
@@ -18013,7 +18013,7 @@
       </c>
       <c r="L395" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M395" t="inlineStr"/>
@@ -18103,7 +18103,7 @@
       </c>
       <c r="L397" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M397" t="inlineStr"/>
@@ -18148,7 +18148,7 @@
       </c>
       <c r="L398" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M398" t="inlineStr"/>
@@ -18234,7 +18234,7 @@
       </c>
       <c r="L400" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M400" t="inlineStr"/>
@@ -18361,7 +18361,7 @@
       </c>
       <c r="L403" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M403" t="inlineStr"/>
@@ -18496,7 +18496,7 @@
       </c>
       <c r="L406" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M406" t="inlineStr"/>
@@ -18541,7 +18541,7 @@
       </c>
       <c r="L407" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M407" t="inlineStr"/>
@@ -18631,7 +18631,7 @@
       </c>
       <c r="L409" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M409" t="inlineStr"/>
@@ -18721,7 +18721,7 @@
       </c>
       <c r="L411" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M411" t="inlineStr"/>
@@ -18811,7 +18811,7 @@
       </c>
       <c r="L413" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M413" t="inlineStr"/>
@@ -18901,7 +18901,7 @@
       </c>
       <c r="L415" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="M415" t="inlineStr"/>
@@ -18946,7 +18946,7 @@
       </c>
       <c r="L416" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M416" t="inlineStr"/>
@@ -18991,7 +18991,7 @@
       </c>
       <c r="L417" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M417" t="inlineStr"/>
@@ -19081,7 +19081,7 @@
       </c>
       <c r="L419" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M419" t="inlineStr"/>
@@ -19171,7 +19171,7 @@
       </c>
       <c r="L421" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M421" t="inlineStr"/>
@@ -19216,7 +19216,7 @@
       </c>
       <c r="L422" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M422" t="inlineStr"/>
@@ -19306,7 +19306,7 @@
       </c>
       <c r="L424" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M424" t="inlineStr"/>
@@ -19351,7 +19351,7 @@
       </c>
       <c r="L425" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M425" t="inlineStr"/>
@@ -19441,7 +19441,7 @@
       </c>
       <c r="L427" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M427" t="inlineStr"/>
@@ -19486,7 +19486,7 @@
       </c>
       <c r="L428" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M428" t="inlineStr"/>
@@ -19576,7 +19576,7 @@
       </c>
       <c r="L430" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M430" t="inlineStr"/>
@@ -19621,7 +19621,7 @@
       </c>
       <c r="L431" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M431" t="inlineStr"/>
@@ -19711,7 +19711,7 @@
       </c>
       <c r="L433" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M433" t="inlineStr"/>
@@ -19756,7 +19756,7 @@
       </c>
       <c r="L434" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M434" t="inlineStr"/>
@@ -19846,7 +19846,7 @@
       </c>
       <c r="L436" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M436" t="inlineStr"/>
@@ -19932,7 +19932,7 @@
       </c>
       <c r="L438" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M438" t="inlineStr"/>
@@ -20067,7 +20067,7 @@
       </c>
       <c r="L441" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M441" t="inlineStr"/>
@@ -20153,7 +20153,7 @@
       </c>
       <c r="L443" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M443" t="inlineStr"/>
@@ -20198,7 +20198,7 @@
       </c>
       <c r="L444" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
       <c r="M444" t="inlineStr"/>
@@ -20460,7 +20460,7 @@
       </c>
       <c r="L450" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M450" t="inlineStr"/>
@@ -20595,7 +20595,7 @@
       </c>
       <c r="L453" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M453" t="inlineStr"/>
@@ -20685,7 +20685,7 @@
       </c>
       <c r="L455" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M455" t="inlineStr"/>
@@ -20857,7 +20857,7 @@
       </c>
       <c r="L459" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M459" t="inlineStr"/>
@@ -20947,7 +20947,7 @@
       </c>
       <c r="L461" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M461" t="inlineStr"/>
@@ -20992,7 +20992,7 @@
       </c>
       <c r="L462" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M462" t="inlineStr"/>
@@ -21209,7 +21209,7 @@
       </c>
       <c r="L467" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="M467" t="inlineStr"/>
@@ -21254,7 +21254,7 @@
       </c>
       <c r="L468" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M468" t="inlineStr"/>
@@ -21385,7 +21385,7 @@
       </c>
       <c r="L471" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M471" t="inlineStr"/>
@@ -21516,7 +21516,7 @@
       </c>
       <c r="L474" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M474" t="inlineStr"/>
@@ -21688,7 +21688,7 @@
       </c>
       <c r="L478" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M478" t="inlineStr"/>
@@ -21823,7 +21823,7 @@
       </c>
       <c r="L481" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M481" t="inlineStr"/>
@@ -22085,7 +22085,7 @@
       </c>
       <c r="L487" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M487" t="inlineStr"/>
@@ -22265,7 +22265,7 @@
       </c>
       <c r="L491" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M491" t="inlineStr"/>
@@ -22310,7 +22310,7 @@
       </c>
       <c r="L492" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M492" t="inlineStr"/>
@@ -22355,7 +22355,7 @@
       </c>
       <c r="L493" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M493" t="inlineStr"/>
@@ -22531,7 +22531,7 @@
       </c>
       <c r="L497" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M497" t="inlineStr"/>
@@ -23108,7 +23108,7 @@
       </c>
       <c r="L510" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M510" t="inlineStr"/>
@@ -24153,7 +24153,7 @@
       </c>
       <c r="L535" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M535" t="inlineStr"/>
@@ -27389,7 +27389,7 @@
       </c>
       <c r="L611" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M611" t="inlineStr"/>
@@ -27434,7 +27434,7 @@
       </c>
       <c r="L612" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
       <c r="M612" t="inlineStr"/>
@@ -31752,7 +31752,7 @@
       </c>
       <c r="L714" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M714" t="inlineStr"/>
@@ -31842,7 +31842,7 @@
       </c>
       <c r="L716" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M716" t="inlineStr"/>
@@ -32059,7 +32059,7 @@
       </c>
       <c r="L721" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="M721" t="inlineStr"/>
@@ -32641,7 +32641,7 @@
       </c>
       <c r="L735" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M735" t="inlineStr"/>
@@ -33190,7 +33190,7 @@
       </c>
       <c r="L748" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M748" t="inlineStr"/>
@@ -33489,7 +33489,7 @@
       </c>
       <c r="L755" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M755" t="inlineStr"/>
@@ -33620,7 +33620,7 @@
       </c>
       <c r="L758" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M758" t="inlineStr"/>
@@ -33796,7 +33796,7 @@
       </c>
       <c r="L762" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M762" t="inlineStr"/>
@@ -35337,7 +35337,7 @@
       </c>
       <c r="L799" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M799" t="inlineStr"/>
@@ -35423,7 +35423,7 @@
       </c>
       <c r="L801" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M801" t="inlineStr"/>
@@ -35800,7 +35800,7 @@
       </c>
       <c r="L810" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M810" t="inlineStr"/>
@@ -36095,7 +36095,7 @@
       </c>
       <c r="L817" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M817" t="inlineStr"/>
@@ -36185,7 +36185,7 @@
       </c>
       <c r="L819" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M819" t="inlineStr"/>
@@ -36316,7 +36316,7 @@
       </c>
       <c r="L822" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M822" t="inlineStr"/>
@@ -36541,7 +36541,7 @@
       </c>
       <c r="L827" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
       <c r="M827" t="inlineStr"/>
@@ -36586,7 +36586,7 @@
       </c>
       <c r="L828" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M828" t="inlineStr"/>
@@ -36672,7 +36672,7 @@
       </c>
       <c r="L830" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M830" t="inlineStr"/>
@@ -36762,7 +36762,7 @@
       </c>
       <c r="L832" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M832" t="inlineStr"/>
@@ -36930,7 +36930,7 @@
       </c>
       <c r="L836" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M836" t="inlineStr"/>
@@ -37110,7 +37110,7 @@
       </c>
       <c r="L840" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M840" t="inlineStr"/>
@@ -37241,7 +37241,7 @@
       </c>
       <c r="L843" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M843" t="inlineStr"/>
@@ -37286,7 +37286,7 @@
       </c>
       <c r="L844" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M844" t="inlineStr"/>
@@ -37372,7 +37372,7 @@
       </c>
       <c r="L846" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M846" t="inlineStr"/>
@@ -37417,7 +37417,7 @@
       </c>
       <c r="L847" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M847" t="inlineStr"/>
@@ -37548,7 +37548,7 @@
       </c>
       <c r="L850" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M850" t="inlineStr"/>
@@ -37724,7 +37724,7 @@
       </c>
       <c r="L854" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
       <c r="M854" t="inlineStr"/>
@@ -37769,7 +37769,7 @@
       </c>
       <c r="L855" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M855" t="inlineStr"/>
@@ -37945,7 +37945,7 @@
       </c>
       <c r="L859" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
       <c r="M859" t="inlineStr"/>
@@ -38031,7 +38031,7 @@
       </c>
       <c r="L861" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M861" t="inlineStr"/>
@@ -38117,7 +38117,7 @@
       </c>
       <c r="L863" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M863" t="inlineStr"/>
@@ -38162,7 +38162,7 @@
       </c>
       <c r="L864" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M864" t="inlineStr"/>
@@ -38248,7 +38248,7 @@
       </c>
       <c r="L866" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M866" t="inlineStr"/>
@@ -38293,7 +38293,7 @@
       </c>
       <c r="L867" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M867" t="inlineStr"/>
@@ -38379,7 +38379,7 @@
       </c>
       <c r="L869" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M869" t="inlineStr"/>
@@ -38424,7 +38424,7 @@
       </c>
       <c r="L870" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M870" t="inlineStr"/>
@@ -38510,7 +38510,7 @@
       </c>
       <c r="L872" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M872" t="inlineStr"/>
@@ -38555,7 +38555,7 @@
       </c>
       <c r="L873" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M873" t="inlineStr"/>
@@ -38641,7 +38641,7 @@
       </c>
       <c r="L875" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M875" t="inlineStr"/>
@@ -38686,7 +38686,7 @@
       </c>
       <c r="L876" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M876" t="inlineStr"/>
@@ -38772,7 +38772,7 @@
       </c>
       <c r="L878" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M878" t="inlineStr"/>
@@ -38817,7 +38817,7 @@
       </c>
       <c r="L879" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M879" t="inlineStr"/>
@@ -38907,7 +38907,7 @@
       </c>
       <c r="L881" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M881" t="inlineStr"/>
@@ -38952,7 +38952,7 @@
       </c>
       <c r="L882" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M882" t="inlineStr"/>
@@ -39038,7 +39038,7 @@
       </c>
       <c r="L884" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M884" t="inlineStr"/>
@@ -39173,7 +39173,7 @@
       </c>
       <c r="L887" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M887" t="inlineStr"/>
@@ -39218,7 +39218,7 @@
       </c>
       <c r="L888" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M888" t="inlineStr"/>
@@ -39304,7 +39304,7 @@
       </c>
       <c r="L890" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M890" t="inlineStr"/>
@@ -39349,7 +39349,7 @@
       </c>
       <c r="L891" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M891" t="inlineStr"/>
@@ -39439,7 +39439,7 @@
       </c>
       <c r="L893" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M893" t="inlineStr"/>
@@ -39648,7 +39648,7 @@
       </c>
       <c r="L898" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M898" t="inlineStr"/>
@@ -39738,7 +39738,7 @@
       </c>
       <c r="L900" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M900" t="inlineStr"/>
@@ -39783,7 +39783,7 @@
       </c>
       <c r="L901" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M901" t="inlineStr"/>
@@ -39869,7 +39869,7 @@
       </c>
       <c r="L903" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M903" t="inlineStr"/>
@@ -40000,7 +40000,7 @@
       </c>
       <c r="L906" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M906" t="inlineStr"/>
@@ -40131,7 +40131,7 @@
       </c>
       <c r="L909" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="M909" t="inlineStr"/>
@@ -40303,7 +40303,7 @@
       </c>
       <c r="L913" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M913" t="inlineStr"/>
@@ -40393,7 +40393,7 @@
       </c>
       <c r="L915" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M915" t="inlineStr"/>
@@ -40573,7 +40573,7 @@
       </c>
       <c r="L919" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M919" t="inlineStr"/>
@@ -40794,7 +40794,7 @@
       </c>
       <c r="L924" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M924" t="inlineStr"/>
@@ -40929,7 +40929,7 @@
       </c>
       <c r="L927" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
       <c r="M927" t="inlineStr"/>
@@ -40974,7 +40974,7 @@
       </c>
       <c r="L928" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M928" t="inlineStr"/>
@@ -41060,7 +41060,7 @@
       </c>
       <c r="L930" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M930" t="inlineStr"/>
@@ -41281,7 +41281,7 @@
       </c>
       <c r="L935" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M935" t="inlineStr"/>
@@ -41502,7 +41502,7 @@
       </c>
       <c r="L940" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M940" t="inlineStr"/>
@@ -41629,7 +41629,7 @@
       </c>
       <c r="L943" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M943" t="inlineStr"/>
@@ -41715,7 +41715,7 @@
       </c>
       <c r="L945" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M945" t="inlineStr"/>
@@ -41760,7 +41760,7 @@
       </c>
       <c r="L946" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M946" t="inlineStr"/>
@@ -41846,7 +41846,7 @@
       </c>
       <c r="L948" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M948" t="inlineStr"/>
@@ -41891,7 +41891,7 @@
       </c>
       <c r="L949" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M949" t="inlineStr"/>
@@ -41977,7 +41977,7 @@
       </c>
       <c r="L951" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M951" t="inlineStr"/>
@@ -42067,7 +42067,7 @@
       </c>
       <c r="L953" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M953" t="inlineStr"/>
@@ -42157,7 +42157,7 @@
       </c>
       <c r="L955" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M955" t="inlineStr"/>
@@ -42202,7 +42202,7 @@
       </c>
       <c r="L956" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M956" t="inlineStr"/>
@@ -42411,7 +42411,7 @@
       </c>
       <c r="L961" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M961" t="inlineStr"/>
@@ -42501,7 +42501,7 @@
       </c>
       <c r="L963" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M963" t="inlineStr"/>
@@ -42628,7 +42628,7 @@
       </c>
       <c r="L966" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M966" t="inlineStr"/>
@@ -42718,7 +42718,7 @@
       </c>
       <c r="L968" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M968" t="inlineStr"/>
@@ -42939,7 +42939,7 @@
       </c>
       <c r="L973" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M973" t="inlineStr"/>
@@ -43025,7 +43025,7 @@
       </c>
       <c r="L975" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M975" t="inlineStr"/>
@@ -43070,7 +43070,7 @@
       </c>
       <c r="L976" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M976" t="inlineStr"/>
@@ -43156,7 +43156,7 @@
       </c>
       <c r="L978" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M978" t="inlineStr"/>
@@ -43246,7 +43246,7 @@
       </c>
       <c r="L980" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M980" t="inlineStr"/>
@@ -43291,7 +43291,7 @@
       </c>
       <c r="L981" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M981" t="inlineStr"/>
@@ -43377,7 +43377,7 @@
       </c>
       <c r="L983" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M983" t="inlineStr"/>
@@ -43422,7 +43422,7 @@
       </c>
       <c r="L984" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M984" t="inlineStr"/>
@@ -43508,7 +43508,7 @@
       </c>
       <c r="L986" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M986" t="inlineStr"/>
@@ -43553,7 +43553,7 @@
       </c>
       <c r="L987" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M987" t="inlineStr"/>
@@ -43639,7 +43639,7 @@
       </c>
       <c r="L989" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M989" t="inlineStr"/>
@@ -43684,7 +43684,7 @@
       </c>
       <c r="L990" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M990" t="inlineStr"/>
@@ -43770,7 +43770,7 @@
       </c>
       <c r="L992" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M992" t="inlineStr"/>
@@ -43815,7 +43815,7 @@
       </c>
       <c r="L993" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M993" t="inlineStr"/>
@@ -43901,7 +43901,7 @@
       </c>
       <c r="L995" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M995" t="inlineStr"/>
@@ -43991,7 +43991,7 @@
       </c>
       <c r="L997" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="M997" t="inlineStr"/>
@@ -44036,7 +44036,7 @@
       </c>
       <c r="L998" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M998" t="inlineStr"/>
@@ -44081,7 +44081,7 @@
       </c>
       <c r="L999" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M999" t="inlineStr"/>
@@ -44167,7 +44167,7 @@
       </c>
       <c r="L1001" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1001" t="inlineStr"/>
@@ -44212,7 +44212,7 @@
       </c>
       <c r="L1002" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1002" t="inlineStr"/>
@@ -44343,7 +44343,7 @@
       </c>
       <c r="L1005" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1005" t="inlineStr"/>
@@ -44388,7 +44388,7 @@
       </c>
       <c r="L1006" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1006" t="inlineStr"/>
@@ -44474,7 +44474,7 @@
       </c>
       <c r="L1008" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1008" t="inlineStr"/>
@@ -44519,7 +44519,7 @@
       </c>
       <c r="L1009" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1009" t="inlineStr"/>
@@ -44605,7 +44605,7 @@
       </c>
       <c r="L1011" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1011" t="inlineStr"/>
@@ -44695,7 +44695,7 @@
       </c>
       <c r="L1013" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1013" t="inlineStr"/>
@@ -44785,7 +44785,7 @@
       </c>
       <c r="L1015" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1015" t="inlineStr"/>
@@ -44912,7 +44912,7 @@
       </c>
       <c r="L1018" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1018" t="inlineStr"/>
@@ -44998,7 +44998,7 @@
       </c>
       <c r="L1020" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1020" t="inlineStr"/>
@@ -45125,7 +45125,7 @@
       </c>
       <c r="L1023" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1023" t="inlineStr"/>
@@ -45211,7 +45211,7 @@
       </c>
       <c r="L1025" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1025" t="inlineStr"/>
@@ -45256,7 +45256,7 @@
       </c>
       <c r="L1026" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1026" t="inlineStr"/>
@@ -45301,7 +45301,7 @@
       </c>
       <c r="L1027" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1027" t="inlineStr"/>
@@ -45391,7 +45391,7 @@
       </c>
       <c r="L1029" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1029" t="inlineStr"/>
@@ -45436,7 +45436,7 @@
       </c>
       <c r="L1030" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="M1030" t="inlineStr"/>
@@ -45567,7 +45567,7 @@
       </c>
       <c r="L1033" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1033" t="inlineStr"/>
@@ -45657,7 +45657,7 @@
       </c>
       <c r="L1035" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1035" t="inlineStr"/>
@@ -45792,7 +45792,7 @@
       </c>
       <c r="L1038" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1038" t="inlineStr"/>
@@ -45837,7 +45837,7 @@
       </c>
       <c r="L1039" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1039" t="inlineStr"/>
@@ -45927,7 +45927,7 @@
       </c>
       <c r="L1041" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1041" t="inlineStr"/>
@@ -45972,7 +45972,7 @@
       </c>
       <c r="L1042" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1042" t="inlineStr"/>
@@ -46062,7 +46062,7 @@
       </c>
       <c r="L1044" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1044" t="inlineStr"/>
@@ -46107,7 +46107,7 @@
       </c>
       <c r="L1045" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1045" t="inlineStr"/>
@@ -46197,7 +46197,7 @@
       </c>
       <c r="L1047" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1047" t="inlineStr"/>
@@ -46242,7 +46242,7 @@
       </c>
       <c r="L1048" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1048" t="inlineStr"/>
@@ -46377,7 +46377,7 @@
       </c>
       <c r="L1051" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1051" t="inlineStr"/>
@@ -46467,7 +46467,7 @@
       </c>
       <c r="L1053" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M1053" t="inlineStr"/>
@@ -46639,7 +46639,7 @@
       </c>
       <c r="L1057" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1057" t="inlineStr"/>
@@ -46684,7 +46684,7 @@
       </c>
       <c r="L1058" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1058" t="inlineStr"/>
@@ -46819,7 +46819,7 @@
       </c>
       <c r="L1061" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1061" t="inlineStr"/>
@@ -46950,7 +46950,7 @@
       </c>
       <c r="L1064" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1064" t="inlineStr"/>
@@ -47085,7 +47085,7 @@
       </c>
       <c r="L1067" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1067" t="inlineStr"/>
@@ -47827,7 +47827,7 @@
       </c>
       <c r="L1085" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1085" t="inlineStr"/>
@@ -47917,7 +47917,7 @@
       </c>
       <c r="L1087" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1087" t="inlineStr"/>
@@ -48089,7 +48089,7 @@
       </c>
       <c r="L1091" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1091" t="inlineStr"/>
@@ -48175,7 +48175,7 @@
       </c>
       <c r="L1093" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1093" t="inlineStr"/>
@@ -48261,7 +48261,7 @@
       </c>
       <c r="L1095" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1095" t="inlineStr"/>
@@ -48351,7 +48351,7 @@
       </c>
       <c r="L1097" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1097" t="inlineStr"/>
@@ -48396,7 +48396,7 @@
       </c>
       <c r="L1098" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1098" t="inlineStr"/>
@@ -48929,7 +48929,7 @@
       </c>
       <c r="L1111" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1111" t="inlineStr"/>
@@ -49019,7 +49019,7 @@
       </c>
       <c r="L1113" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1113" t="inlineStr"/>
@@ -49064,7 +49064,7 @@
       </c>
       <c r="L1114" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1114" t="inlineStr"/>
@@ -49154,7 +49154,7 @@
       </c>
       <c r="L1116" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1116" t="inlineStr"/>
@@ -49199,7 +49199,7 @@
       </c>
       <c r="L1117" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="M1117" t="inlineStr"/>
@@ -49330,7 +49330,7 @@
       </c>
       <c r="L1120" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="M1120" t="inlineStr"/>
@@ -49461,7 +49461,7 @@
       </c>
       <c r="L1123" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1123" t="inlineStr"/>
@@ -49547,7 +49547,7 @@
       </c>
       <c r="L1125" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1125" t="inlineStr"/>
@@ -49592,7 +49592,7 @@
       </c>
       <c r="L1126" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
       <c r="M1126" t="inlineStr"/>
@@ -49637,7 +49637,7 @@
       </c>
       <c r="L1127" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1127" t="inlineStr"/>
@@ -49805,7 +49805,7 @@
       </c>
       <c r="L1131" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1131" t="inlineStr"/>
@@ -49891,7 +49891,7 @@
       </c>
       <c r="L1133" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1133" t="inlineStr"/>
@@ -50018,7 +50018,7 @@
       </c>
       <c r="L1136" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1136" t="inlineStr"/>
@@ -50108,7 +50108,7 @@
       </c>
       <c r="L1138" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1138" t="inlineStr"/>
@@ -50153,7 +50153,7 @@
       </c>
       <c r="L1139" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1139" t="inlineStr"/>
@@ -50243,7 +50243,7 @@
       </c>
       <c r="L1141" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1141" t="inlineStr"/>
@@ -50288,7 +50288,7 @@
       </c>
       <c r="L1142" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1142" t="inlineStr"/>
@@ -50333,7 +50333,7 @@
       </c>
       <c r="L1143" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1143" t="inlineStr"/>
@@ -50378,7 +50378,7 @@
       </c>
       <c r="L1144" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1144" t="inlineStr"/>
@@ -50423,7 +50423,7 @@
       </c>
       <c r="L1145" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1145" t="inlineStr"/>
@@ -50718,7 +50718,7 @@
       </c>
       <c r="L1152" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1152" t="inlineStr"/>
@@ -50849,7 +50849,7 @@
       </c>
       <c r="L1155" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M1155" t="inlineStr"/>
@@ -50976,7 +50976,7 @@
       </c>
       <c r="L1158" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1158" t="inlineStr"/>
@@ -51062,7 +51062,7 @@
       </c>
       <c r="L1160" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1160" t="inlineStr"/>
@@ -51107,7 +51107,7 @@
       </c>
       <c r="L1161" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1161" t="inlineStr"/>
@@ -51193,7 +51193,7 @@
       </c>
       <c r="L1163" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1163" t="inlineStr"/>
@@ -51328,7 +51328,7 @@
       </c>
       <c r="L1166" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1166" t="inlineStr"/>
@@ -51373,7 +51373,7 @@
       </c>
       <c r="L1167" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1167" t="inlineStr"/>
@@ -51459,7 +51459,7 @@
       </c>
       <c r="L1169" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1169" t="inlineStr"/>
@@ -51504,7 +51504,7 @@
       </c>
       <c r="L1170" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1170" t="inlineStr"/>
@@ -51590,7 +51590,7 @@
       </c>
       <c r="L1172" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1172" t="inlineStr"/>
@@ -51680,7 +51680,7 @@
       </c>
       <c r="L1174" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1174" t="inlineStr"/>
@@ -51725,7 +51725,7 @@
       </c>
       <c r="L1175" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1175" t="inlineStr"/>
@@ -51811,7 +51811,7 @@
       </c>
       <c r="L1177" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1177" t="inlineStr"/>
@@ -51901,7 +51901,7 @@
       </c>
       <c r="L1179" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1179" t="inlineStr"/>
@@ -52352,7 +52352,7 @@
       </c>
       <c r="L1190" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1190" t="inlineStr"/>
@@ -52442,7 +52442,7 @@
       </c>
       <c r="L1192" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1192" t="inlineStr"/>
@@ -52614,7 +52614,7 @@
       </c>
       <c r="L1196" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1196" t="inlineStr"/>
@@ -52704,7 +52704,7 @@
       </c>
       <c r="L1198" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1198" t="inlineStr"/>
@@ -52749,7 +52749,7 @@
       </c>
       <c r="L1199" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1199" t="inlineStr"/>
@@ -52839,7 +52839,7 @@
       </c>
       <c r="L1201" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1201" t="inlineStr"/>
@@ -52884,7 +52884,7 @@
       </c>
       <c r="L1202" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1202" t="inlineStr"/>
@@ -53015,7 +53015,7 @@
       </c>
       <c r="L1205" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1205" t="inlineStr"/>
@@ -53060,7 +53060,7 @@
       </c>
       <c r="L1206" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
       <c r="M1206" t="inlineStr"/>
@@ -53236,7 +53236,7 @@
       </c>
       <c r="L1210" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1210" t="inlineStr"/>
@@ -53367,7 +53367,7 @@
       </c>
       <c r="L1213" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1213" t="inlineStr"/>
@@ -53457,7 +53457,7 @@
       </c>
       <c r="L1215" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="M1215" t="inlineStr"/>
@@ -53502,7 +53502,7 @@
       </c>
       <c r="L1216" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1216" t="inlineStr"/>
@@ -53629,7 +53629,7 @@
       </c>
       <c r="L1219" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1219" t="inlineStr"/>
@@ -53674,7 +53674,7 @@
       </c>
       <c r="L1220" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1220" t="inlineStr"/>
@@ -53719,7 +53719,7 @@
       </c>
       <c r="L1221" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1221" t="inlineStr"/>
@@ -53764,7 +53764,7 @@
       </c>
       <c r="L1222" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1222" t="inlineStr"/>
@@ -53809,7 +53809,7 @@
       </c>
       <c r="L1223" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1223" t="inlineStr"/>
@@ -53940,7 +53940,7 @@
       </c>
       <c r="L1226" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1226" t="inlineStr"/>
@@ -54030,7 +54030,7 @@
       </c>
       <c r="L1228" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1228" t="inlineStr"/>
@@ -54366,7 +54366,7 @@
       </c>
       <c r="L1236" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1236" t="inlineStr"/>
@@ -54411,7 +54411,7 @@
       </c>
       <c r="L1237" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1237" t="inlineStr"/>
@@ -54501,7 +54501,7 @@
       </c>
       <c r="L1239" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1239" t="inlineStr"/>
@@ -54636,7 +54636,7 @@
       </c>
       <c r="L1242" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1242" t="inlineStr"/>
@@ -54722,7 +54722,7 @@
       </c>
       <c r="L1244" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1244" t="inlineStr"/>
@@ -54767,7 +54767,7 @@
       </c>
       <c r="L1245" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1245" t="inlineStr"/>
@@ -54853,7 +54853,7 @@
       </c>
       <c r="L1247" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1247" t="inlineStr"/>
@@ -54898,7 +54898,7 @@
       </c>
       <c r="L1248" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1248" t="inlineStr"/>
@@ -54984,7 +54984,7 @@
       </c>
       <c r="L1250" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1250" t="inlineStr"/>
@@ -55029,7 +55029,7 @@
       </c>
       <c r="L1251" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1251" t="inlineStr"/>
@@ -55115,7 +55115,7 @@
       </c>
       <c r="L1253" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1253" t="inlineStr"/>
@@ -55160,7 +55160,7 @@
       </c>
       <c r="L1254" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1254" t="inlineStr"/>
@@ -55246,7 +55246,7 @@
       </c>
       <c r="L1256" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1256" t="inlineStr"/>
@@ -55291,7 +55291,7 @@
       </c>
       <c r="L1257" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1257" t="inlineStr"/>
@@ -55377,7 +55377,7 @@
       </c>
       <c r="L1259" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1259" t="inlineStr"/>
@@ -55422,7 +55422,7 @@
       </c>
       <c r="L1260" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1260" t="inlineStr"/>
@@ -55508,7 +55508,7 @@
       </c>
       <c r="L1262" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1262" t="inlineStr"/>
@@ -55553,7 +55553,7 @@
       </c>
       <c r="L1263" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1263" t="inlineStr"/>
@@ -55643,7 +55643,7 @@
       </c>
       <c r="L1265" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1265" t="inlineStr"/>
@@ -55688,7 +55688,7 @@
       </c>
       <c r="L1266" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1266" t="inlineStr"/>
@@ -55774,7 +55774,7 @@
       </c>
       <c r="L1268" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1268" t="inlineStr"/>
@@ -55819,7 +55819,7 @@
       </c>
       <c r="L1269" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1269" t="inlineStr"/>
@@ -55905,7 +55905,7 @@
       </c>
       <c r="L1271" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1271" t="inlineStr"/>
@@ -55995,7 +55995,7 @@
       </c>
       <c r="L1273" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1273" t="inlineStr"/>
@@ -56040,7 +56040,7 @@
       </c>
       <c r="L1274" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1274" t="inlineStr"/>
@@ -56126,7 +56126,7 @@
       </c>
       <c r="L1276" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1276" t="inlineStr"/>
@@ -56298,7 +56298,7 @@
       </c>
       <c r="L1280" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
       <c r="M1280" t="inlineStr"/>
@@ -56384,7 +56384,7 @@
       </c>
       <c r="L1282" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1282" t="inlineStr"/>
@@ -56429,7 +56429,7 @@
       </c>
       <c r="L1283" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1283" t="inlineStr"/>
@@ -56515,7 +56515,7 @@
       </c>
       <c r="L1285" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1285" t="inlineStr"/>
@@ -56605,7 +56605,7 @@
       </c>
       <c r="L1287" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1287" t="inlineStr"/>
@@ -56732,7 +56732,7 @@
       </c>
       <c r="L1290" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
       <c r="M1290" t="inlineStr"/>
@@ -56990,7 +56990,7 @@
       </c>
       <c r="L1296" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1296" t="inlineStr"/>
@@ -57121,7 +57121,7 @@
       </c>
       <c r="L1299" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1299" t="inlineStr"/>
@@ -57412,7 +57412,7 @@
       </c>
       <c r="L1306" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1306" t="inlineStr"/>
@@ -57502,7 +57502,7 @@
       </c>
       <c r="L1308" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1308" t="inlineStr"/>
@@ -57588,7 +57588,7 @@
       </c>
       <c r="L1310" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1310" t="inlineStr"/>
@@ -57674,7 +57674,7 @@
       </c>
       <c r="L1312" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
       <c r="M1312" t="inlineStr"/>
@@ -57838,7 +57838,7 @@
       </c>
       <c r="L1316" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1316" t="inlineStr"/>
@@ -57924,7 +57924,7 @@
       </c>
       <c r="L1318" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1318" t="inlineStr"/>
@@ -58014,7 +58014,7 @@
       </c>
       <c r="L1320" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1320" t="inlineStr"/>
@@ -58059,7 +58059,7 @@
       </c>
       <c r="L1321" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1321" t="inlineStr"/>
@@ -58149,7 +58149,7 @@
       </c>
       <c r="L1323" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1323" t="inlineStr"/>
@@ -58239,7 +58239,7 @@
       </c>
       <c r="L1325" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1325" t="inlineStr"/>
@@ -58325,7 +58325,7 @@
       </c>
       <c r="L1327" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1327" t="inlineStr"/>
@@ -58411,7 +58411,7 @@
       </c>
       <c r="L1329" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1329" t="inlineStr"/>
@@ -58497,7 +58497,7 @@
       </c>
       <c r="L1331" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1331" t="inlineStr"/>
@@ -58583,7 +58583,7 @@
       </c>
       <c r="L1333" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1333" t="inlineStr"/>
@@ -58669,7 +58669,7 @@
       </c>
       <c r="L1335" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1335" t="inlineStr"/>
@@ -58759,7 +58759,7 @@
       </c>
       <c r="L1337" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1337" t="inlineStr"/>
@@ -58849,7 +58849,7 @@
       </c>
       <c r="L1339" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1339" t="inlineStr"/>
@@ -58894,7 +58894,7 @@
       </c>
       <c r="L1340" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1340" t="inlineStr"/>
@@ -58980,7 +58980,7 @@
       </c>
       <c r="L1342" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1342" t="inlineStr"/>
@@ -59115,7 +59115,7 @@
       </c>
       <c r="L1345" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1345" t="inlineStr"/>
@@ -59250,7 +59250,7 @@
       </c>
       <c r="L1348" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1348" t="inlineStr"/>
@@ -59340,7 +59340,7 @@
       </c>
       <c r="L1350" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1350" t="inlineStr"/>
@@ -59385,7 +59385,7 @@
       </c>
       <c r="L1351" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M1351" t="inlineStr"/>
@@ -59512,7 +59512,7 @@
       </c>
       <c r="L1354" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1354" t="inlineStr"/>
@@ -59598,7 +59598,7 @@
       </c>
       <c r="L1356" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1356" t="inlineStr"/>
@@ -59643,7 +59643,7 @@
       </c>
       <c r="L1357" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1357" t="inlineStr"/>
@@ -59774,7 +59774,7 @@
       </c>
       <c r="L1360" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1360" t="inlineStr"/>
@@ -59819,7 +59819,7 @@
       </c>
       <c r="L1361" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1361" t="inlineStr"/>
@@ -59905,7 +59905,7 @@
       </c>
       <c r="L1363" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1363" t="inlineStr"/>
@@ -59950,7 +59950,7 @@
       </c>
       <c r="L1364" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1364" t="inlineStr"/>
@@ -60036,7 +60036,7 @@
       </c>
       <c r="L1366" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1366" t="inlineStr"/>
@@ -60126,7 +60126,7 @@
       </c>
       <c r="L1368" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1368" t="inlineStr"/>
@@ -60212,7 +60212,7 @@
       </c>
       <c r="L1370" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1370" t="inlineStr"/>
@@ -60302,7 +60302,7 @@
       </c>
       <c r="L1372" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1372" t="inlineStr"/>
@@ -60347,7 +60347,7 @@
       </c>
       <c r="L1373" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
       <c r="M1373" t="inlineStr"/>
@@ -60478,7 +60478,7 @@
       </c>
       <c r="L1376" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1376" t="inlineStr"/>
@@ -60568,7 +60568,7 @@
       </c>
       <c r="L1378" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1378" t="inlineStr"/>
@@ -60613,7 +60613,7 @@
       </c>
       <c r="L1379" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1379" t="inlineStr"/>
@@ -60744,7 +60744,7 @@
       </c>
       <c r="L1382" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1382" t="inlineStr"/>
@@ -60830,7 +60830,7 @@
       </c>
       <c r="L1384" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1384" t="inlineStr"/>
@@ -60965,7 +60965,7 @@
       </c>
       <c r="L1387" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1387" t="inlineStr"/>
@@ -61010,7 +61010,7 @@
       </c>
       <c r="L1388" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1388" t="inlineStr"/>
@@ -61096,7 +61096,7 @@
       </c>
       <c r="L1390" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1390" t="inlineStr"/>
@@ -61141,7 +61141,7 @@
       </c>
       <c r="L1391" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
       <c r="M1391" t="inlineStr"/>
@@ -61186,7 +61186,7 @@
       </c>
       <c r="L1392" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1392" t="inlineStr"/>
@@ -61276,7 +61276,7 @@
       </c>
       <c r="L1394" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
       <c r="M1394" t="inlineStr"/>
@@ -61321,7 +61321,7 @@
       </c>
       <c r="L1395" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
       <c r="M1395" t="inlineStr"/>
@@ -61407,7 +61407,7 @@
       </c>
       <c r="L1397" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1397" t="inlineStr"/>
@@ -61497,7 +61497,7 @@
       </c>
       <c r="L1399" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1399" t="inlineStr"/>
@@ -61542,7 +61542,7 @@
       </c>
       <c r="L1400" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1400" t="inlineStr"/>
@@ -61632,7 +61632,7 @@
       </c>
       <c r="L1402" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1402" t="inlineStr"/>
@@ -61804,7 +61804,7 @@
       </c>
       <c r="L1406" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
       <c r="M1406" t="inlineStr"/>
@@ -61849,7 +61849,7 @@
       </c>
       <c r="L1407" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1407" t="inlineStr"/>
@@ -61894,7 +61894,7 @@
       </c>
       <c r="L1408" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
       <c r="M1408" t="inlineStr"/>
@@ -61980,7 +61980,7 @@
       </c>
       <c r="L1410" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1410" t="inlineStr"/>
@@ -62156,7 +62156,7 @@
       </c>
       <c r="L1414" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
       <c r="M1414" t="inlineStr"/>

</xml_diff>

<commit_message>
reconcile 84000 ids, factor out numbers for roles
</commit_message>
<xml_diff>
--- a/WD_BDRC_data.xlsx
+++ b/WD_BDRC_data.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -748,7 +748,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -797,7 +797,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -895,7 +895,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -944,7 +944,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1185,7 +1185,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1234,7 +1234,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -1430,7 +1430,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -1524,7 +1524,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -1667,7 +1667,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -1716,7 +1716,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -1908,7 +1908,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
@@ -2484,7 +2484,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
@@ -2631,7 +2631,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
@@ -2778,7 +2778,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
@@ -2925,7 +2925,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
@@ -3072,7 +3072,7 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
@@ -3170,7 +3170,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M59" t="inlineStr">
@@ -3452,7 +3452,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M62" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M63" t="inlineStr">
@@ -3599,7 +3599,7 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M65" t="inlineStr">
@@ -3697,7 +3697,7 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M67" t="inlineStr">
@@ -3795,7 +3795,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M69" t="inlineStr">
@@ -3893,7 +3893,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
@@ -3942,7 +3942,7 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M72" t="inlineStr">
@@ -3991,7 +3991,7 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M73" t="inlineStr">
@@ -4040,7 +4040,7 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M74" t="inlineStr">
@@ -4089,7 +4089,7 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M75" t="inlineStr">
@@ -4138,7 +4138,7 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M76" t="inlineStr">
@@ -4187,7 +4187,7 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M77" t="inlineStr">
@@ -4285,7 +4285,7 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M79" t="inlineStr">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -4481,7 +4481,7 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -4530,7 +4530,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -4628,7 +4628,7 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M86" t="inlineStr">
@@ -4775,7 +4775,7 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M89" t="inlineStr">
@@ -4873,7 +4873,7 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M91" t="inlineStr">
@@ -4922,7 +4922,7 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M92" t="inlineStr">
@@ -5020,7 +5020,7 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M94" t="inlineStr">
@@ -5167,7 +5167,7 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M97" t="inlineStr">
@@ -5265,7 +5265,7 @@
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
       <c r="M99" t="inlineStr">
@@ -5686,7 +5686,7 @@
       </c>
       <c r="L108" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M108" t="inlineStr">
@@ -5931,7 +5931,7 @@
       </c>
       <c r="L113" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M113" t="inlineStr">
@@ -6078,7 +6078,7 @@
       </c>
       <c r="L116" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M116" t="inlineStr">
@@ -6274,7 +6274,7 @@
       </c>
       <c r="L120" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M120" t="inlineStr">
@@ -6323,7 +6323,7 @@
       </c>
       <c r="L121" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M121" t="inlineStr">
@@ -6421,7 +6421,7 @@
       </c>
       <c r="L123" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M123" t="inlineStr">
@@ -6519,7 +6519,7 @@
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M125" t="inlineStr">
@@ -6617,7 +6617,7 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M127" t="inlineStr">
@@ -6666,7 +6666,7 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M128" t="inlineStr">
@@ -6715,7 +6715,7 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
       <c r="M129" t="inlineStr">
@@ -6813,7 +6813,7 @@
       </c>
       <c r="L131" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M131" t="inlineStr">
@@ -7107,7 +7107,7 @@
       </c>
       <c r="L137" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M137" t="inlineStr">
@@ -7156,7 +7156,7 @@
       </c>
       <c r="L138" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M138" t="inlineStr">
@@ -7254,7 +7254,7 @@
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M140" t="inlineStr">
@@ -7303,7 +7303,7 @@
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M141" t="inlineStr">
@@ -7401,7 +7401,7 @@
       </c>
       <c r="L143" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M143" t="inlineStr">
@@ -7499,7 +7499,7 @@
       </c>
       <c r="L145" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M145" t="inlineStr">
@@ -7548,7 +7548,7 @@
       </c>
       <c r="L146" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M146" t="inlineStr">
@@ -7597,7 +7597,7 @@
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M147" t="inlineStr">
@@ -7695,7 +7695,7 @@
       </c>
       <c r="L149" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M149" t="inlineStr">
@@ -7744,7 +7744,7 @@
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M150" t="inlineStr">
@@ -7842,7 +7842,7 @@
       </c>
       <c r="L152" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M152" t="inlineStr">
@@ -7940,7 +7940,7 @@
       </c>
       <c r="L154" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M154" t="inlineStr">
@@ -8038,7 +8038,7 @@
       </c>
       <c r="L156" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M156" t="inlineStr">
@@ -8185,7 +8185,7 @@
       </c>
       <c r="L159" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M159" t="inlineStr">
@@ -8377,7 +8377,7 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M163" t="inlineStr">
@@ -8426,7 +8426,7 @@
       </c>
       <c r="L164" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M164" t="inlineStr">
@@ -8573,7 +8573,7 @@
       </c>
       <c r="L167" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M167" t="inlineStr">
@@ -8622,7 +8622,7 @@
       </c>
       <c r="L168" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M168" t="inlineStr">
@@ -8720,7 +8720,7 @@
       </c>
       <c r="L170" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M170" t="inlineStr">
@@ -8769,7 +8769,7 @@
       </c>
       <c r="L171" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M171" t="inlineStr">
@@ -8867,7 +8867,7 @@
       </c>
       <c r="L173" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
       <c r="M173" t="inlineStr">
@@ -8916,7 +8916,7 @@
       </c>
       <c r="L174" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M174" t="inlineStr">
@@ -9014,7 +9014,7 @@
       </c>
       <c r="L176" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M176" t="inlineStr">
@@ -9063,7 +9063,7 @@
       </c>
       <c r="L177" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M177" t="inlineStr">
@@ -9161,7 +9161,7 @@
       </c>
       <c r="L179" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="M179" t="inlineStr">
@@ -9210,7 +9210,7 @@
       </c>
       <c r="L180" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M180" t="inlineStr">
@@ -9259,7 +9259,7 @@
       </c>
       <c r="L181" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M181" t="inlineStr">
@@ -9308,7 +9308,7 @@
       </c>
       <c r="L182" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M182" t="inlineStr">
@@ -9455,7 +9455,7 @@
       </c>
       <c r="L185" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M185" t="inlineStr">
@@ -9602,7 +9602,7 @@
       </c>
       <c r="L188" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M188" t="inlineStr">
@@ -9749,7 +9749,7 @@
       </c>
       <c r="L191" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M191" t="inlineStr">
@@ -9896,7 +9896,7 @@
       </c>
       <c r="L194" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M194" t="inlineStr">
@@ -9994,7 +9994,7 @@
       </c>
       <c r="L196" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M196" t="inlineStr">
@@ -10043,7 +10043,7 @@
       </c>
       <c r="L197" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M197" t="inlineStr">
@@ -10288,7 +10288,7 @@
       </c>
       <c r="L202" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M202" t="inlineStr">
@@ -10337,7 +10337,7 @@
       </c>
       <c r="L203" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M203" t="inlineStr">
@@ -10386,7 +10386,7 @@
       </c>
       <c r="L204" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M204" t="inlineStr">
@@ -10484,7 +10484,7 @@
       </c>
       <c r="L206" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M206" t="inlineStr">
@@ -10533,7 +10533,7 @@
       </c>
       <c r="L207" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M207" t="inlineStr">
@@ -10631,7 +10631,7 @@
       </c>
       <c r="L209" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M209" t="inlineStr">
@@ -10778,7 +10778,7 @@
       </c>
       <c r="L212" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M212" t="inlineStr">
@@ -10827,7 +10827,7 @@
       </c>
       <c r="L213" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M213" t="inlineStr">
@@ -10925,7 +10925,7 @@
       </c>
       <c r="L215" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M215" t="inlineStr">
@@ -11219,7 +11219,7 @@
       </c>
       <c r="L221" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M221" t="inlineStr">
@@ -11268,7 +11268,7 @@
       </c>
       <c r="L222" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M222" t="inlineStr">
@@ -11317,7 +11317,7 @@
       </c>
       <c r="L223" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
       <c r="M223" t="inlineStr">
@@ -11366,7 +11366,7 @@
       </c>
       <c r="L224" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M224" t="inlineStr">
@@ -11464,7 +11464,7 @@
       </c>
       <c r="L226" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M226" t="inlineStr">
@@ -11611,7 +11611,7 @@
       </c>
       <c r="L229" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M229" t="inlineStr">
@@ -11660,7 +11660,7 @@
       </c>
       <c r="L230" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M230" t="inlineStr">
@@ -11758,7 +11758,7 @@
       </c>
       <c r="L232" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M232" t="inlineStr">
@@ -11856,7 +11856,7 @@
       </c>
       <c r="L234" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M234" t="inlineStr">
@@ -11905,7 +11905,7 @@
       </c>
       <c r="L235" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M235" t="inlineStr">
@@ -12003,7 +12003,7 @@
       </c>
       <c r="L237" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M237" t="inlineStr">
@@ -12101,7 +12101,7 @@
       </c>
       <c r="L239" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M239" t="inlineStr">
@@ -12538,7 +12538,7 @@
       </c>
       <c r="L248" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M248" t="inlineStr">
@@ -12587,7 +12587,7 @@
       </c>
       <c r="L249" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M249" t="inlineStr">
@@ -12636,7 +12636,7 @@
       </c>
       <c r="L250" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M250" t="inlineStr">
@@ -12734,7 +12734,7 @@
       </c>
       <c r="L252" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M252" t="inlineStr">
@@ -12832,7 +12832,7 @@
       </c>
       <c r="L254" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M254" t="inlineStr">
@@ -12930,7 +12930,7 @@
       </c>
       <c r="L256" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M256" t="inlineStr">
@@ -13028,7 +13028,7 @@
       </c>
       <c r="L258" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M258" t="inlineStr">
@@ -13126,7 +13126,7 @@
       </c>
       <c r="L260" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M260" t="inlineStr">
@@ -13265,7 +13265,7 @@
       </c>
       <c r="L263" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M263" t="inlineStr">
@@ -13363,7 +13363,7 @@
       </c>
       <c r="L265" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M265" t="inlineStr">
@@ -13461,7 +13461,7 @@
       </c>
       <c r="L267" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M267" t="inlineStr">
@@ -13559,7 +13559,7 @@
       </c>
       <c r="L269" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M269" t="inlineStr">
@@ -13706,7 +13706,7 @@
       </c>
       <c r="L272" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M272" t="inlineStr">
@@ -13902,7 +13902,7 @@
       </c>
       <c r="L276" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M276" t="inlineStr">
@@ -14290,7 +14290,7 @@
       </c>
       <c r="L284" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M284" t="inlineStr">
@@ -14613,7 +14613,7 @@
       </c>
       <c r="L291" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M291" t="inlineStr">
@@ -14854,7 +14854,7 @@
       </c>
       <c r="L296" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M296" t="inlineStr">
@@ -14952,7 +14952,7 @@
       </c>
       <c r="L298" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M298" t="inlineStr">
@@ -15001,7 +15001,7 @@
       </c>
       <c r="L299" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M299" t="inlineStr">
@@ -15099,7 +15099,7 @@
       </c>
       <c r="L301" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M301" t="inlineStr">
@@ -15148,7 +15148,7 @@
       </c>
       <c r="L302" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M302" t="inlineStr">
@@ -15246,7 +15246,7 @@
       </c>
       <c r="L304" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M304" t="inlineStr">
@@ -15295,7 +15295,7 @@
       </c>
       <c r="L305" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M305" t="inlineStr">
@@ -15393,7 +15393,7 @@
       </c>
       <c r="L307" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M307" t="inlineStr">
@@ -15487,7 +15487,7 @@
       </c>
       <c r="L309" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="M309" t="inlineStr">
@@ -15581,7 +15581,7 @@
       </c>
       <c r="L311" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M311" t="inlineStr">
@@ -15679,7 +15679,7 @@
       </c>
       <c r="L313" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M313" t="inlineStr">
@@ -15777,7 +15777,7 @@
       </c>
       <c r="L315" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="M315" t="inlineStr">
@@ -15826,7 +15826,7 @@
       </c>
       <c r="L316" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M316" t="inlineStr">
@@ -15924,7 +15924,7 @@
       </c>
       <c r="L318" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M318" t="inlineStr">
@@ -16071,7 +16071,7 @@
       </c>
       <c r="L321" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M321" t="inlineStr">
@@ -16120,7 +16120,7 @@
       </c>
       <c r="L322" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
       <c r="M322" t="inlineStr">
@@ -16169,7 +16169,7 @@
       </c>
       <c r="L323" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M323" t="inlineStr">
@@ -16218,7 +16218,7 @@
       </c>
       <c r="L324" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M324" t="inlineStr">
@@ -16316,7 +16316,7 @@
       </c>
       <c r="L326" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M326" t="inlineStr">
@@ -16365,7 +16365,7 @@
       </c>
       <c r="L327" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M327" t="inlineStr">
@@ -16414,7 +16414,7 @@
       </c>
       <c r="L328" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
       <c r="M328" t="inlineStr">
@@ -16463,7 +16463,7 @@
       </c>
       <c r="L329" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M329" t="inlineStr">
@@ -16561,7 +16561,7 @@
       </c>
       <c r="L331" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M331" t="inlineStr">
@@ -16708,7 +16708,7 @@
       </c>
       <c r="L334" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M334" t="inlineStr">
@@ -16757,7 +16757,7 @@
       </c>
       <c r="L335" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
       <c r="M335" t="inlineStr">
@@ -16806,7 +16806,7 @@
       </c>
       <c r="L336" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M336" t="inlineStr">
@@ -17002,7 +17002,7 @@
       </c>
       <c r="L340" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M340" t="inlineStr">
@@ -17100,7 +17100,7 @@
       </c>
       <c r="L342" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M342" t="inlineStr">
@@ -17149,7 +17149,7 @@
       </c>
       <c r="L343" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M343" t="inlineStr">
@@ -17247,7 +17247,7 @@
       </c>
       <c r="L345" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M345" t="inlineStr">
@@ -17296,7 +17296,7 @@
       </c>
       <c r="L346" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M346" t="inlineStr">
@@ -17394,7 +17394,7 @@
       </c>
       <c r="L348" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M348" t="inlineStr">
@@ -17590,7 +17590,7 @@
       </c>
       <c r="L352" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M352" t="inlineStr">
@@ -17737,7 +17737,7 @@
       </c>
       <c r="L355" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M355" t="inlineStr">
@@ -17835,7 +17835,7 @@
       </c>
       <c r="L357" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
       <c r="M357" t="inlineStr">
@@ -17884,7 +17884,7 @@
       </c>
       <c r="L358" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M358" t="inlineStr">
@@ -18031,7 +18031,7 @@
       </c>
       <c r="L361" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M361" t="inlineStr">
@@ -18129,7 +18129,7 @@
       </c>
       <c r="L363" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M363" t="inlineStr">
@@ -18178,7 +18178,7 @@
       </c>
       <c r="L364" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M364" t="inlineStr">
@@ -18276,7 +18276,7 @@
       </c>
       <c r="L366" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M366" t="inlineStr">
@@ -18325,7 +18325,7 @@
       </c>
       <c r="L367" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M367" t="inlineStr">
@@ -18423,7 +18423,7 @@
       </c>
       <c r="L369" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M369" t="inlineStr">
@@ -18660,7 +18660,7 @@
       </c>
       <c r="L374" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M374" t="inlineStr">
@@ -18709,7 +18709,7 @@
       </c>
       <c r="L375" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M375" t="inlineStr">
@@ -18807,7 +18807,7 @@
       </c>
       <c r="L377" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M377" t="inlineStr">
@@ -18856,7 +18856,7 @@
       </c>
       <c r="L378" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
       <c r="M378" t="inlineStr">
@@ -19097,7 +19097,7 @@
       </c>
       <c r="L383" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M383" t="inlineStr">
@@ -19146,7 +19146,7 @@
       </c>
       <c r="L384" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M384" t="inlineStr">
@@ -19244,7 +19244,7 @@
       </c>
       <c r="L386" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
       <c r="M386" t="inlineStr">
@@ -19293,7 +19293,7 @@
       </c>
       <c r="L387" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M387" t="inlineStr">
@@ -19583,7 +19583,7 @@
       </c>
       <c r="L393" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M393" t="inlineStr">
@@ -19681,7 +19681,7 @@
       </c>
       <c r="L395" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M395" t="inlineStr">
@@ -19779,7 +19779,7 @@
       </c>
       <c r="L397" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M397" t="inlineStr">
@@ -19828,7 +19828,7 @@
       </c>
       <c r="L398" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M398" t="inlineStr">
@@ -19926,7 +19926,7 @@
       </c>
       <c r="L400" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M400" t="inlineStr">
@@ -20065,7 +20065,7 @@
       </c>
       <c r="L403" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M403" t="inlineStr">
@@ -20212,7 +20212,7 @@
       </c>
       <c r="L406" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M406" t="inlineStr">
@@ -20261,7 +20261,7 @@
       </c>
       <c r="L407" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M407" t="inlineStr">
@@ -20359,7 +20359,7 @@
       </c>
       <c r="L409" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M409" t="inlineStr">
@@ -20457,7 +20457,7 @@
       </c>
       <c r="L411" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M411" t="inlineStr">
@@ -20555,7 +20555,7 @@
       </c>
       <c r="L413" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M413" t="inlineStr">
@@ -20653,7 +20653,7 @@
       </c>
       <c r="L415" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M415" t="inlineStr">
@@ -20702,7 +20702,7 @@
       </c>
       <c r="L416" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M416" t="inlineStr">
@@ -20751,7 +20751,7 @@
       </c>
       <c r="L417" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M417" t="inlineStr">
@@ -20849,7 +20849,7 @@
       </c>
       <c r="L419" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M419" t="inlineStr">
@@ -20947,7 +20947,7 @@
       </c>
       <c r="L421" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M421" t="inlineStr">
@@ -20996,7 +20996,7 @@
       </c>
       <c r="L422" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M422" t="inlineStr">
@@ -21094,7 +21094,7 @@
       </c>
       <c r="L424" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M424" t="inlineStr">
@@ -21143,7 +21143,7 @@
       </c>
       <c r="L425" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M425" t="inlineStr">
@@ -21241,7 +21241,7 @@
       </c>
       <c r="L427" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M427" t="inlineStr">
@@ -21290,7 +21290,7 @@
       </c>
       <c r="L428" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M428" t="inlineStr">
@@ -21388,7 +21388,7 @@
       </c>
       <c r="L430" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M430" t="inlineStr">
@@ -21437,7 +21437,7 @@
       </c>
       <c r="L431" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M431" t="inlineStr">
@@ -21535,7 +21535,7 @@
       </c>
       <c r="L433" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M433" t="inlineStr">
@@ -21584,7 +21584,7 @@
       </c>
       <c r="L434" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M434" t="inlineStr">
@@ -21682,7 +21682,7 @@
       </c>
       <c r="L436" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M436" t="inlineStr">
@@ -21776,7 +21776,7 @@
       </c>
       <c r="L438" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M438" t="inlineStr">
@@ -22017,7 +22017,7 @@
       </c>
       <c r="L443" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M443" t="inlineStr">
@@ -22352,7 +22352,7 @@
       </c>
       <c r="L450" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M450" t="inlineStr">
@@ -22499,7 +22499,7 @@
       </c>
       <c r="L453" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M453" t="inlineStr">
@@ -22597,7 +22597,7 @@
       </c>
       <c r="L455" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M455" t="inlineStr">
@@ -22785,7 +22785,7 @@
       </c>
       <c r="L459" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M459" t="inlineStr">
@@ -22883,7 +22883,7 @@
       </c>
       <c r="L461" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M461" t="inlineStr">
@@ -22932,7 +22932,7 @@
       </c>
       <c r="L462" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M462" t="inlineStr">
@@ -23169,7 +23169,7 @@
       </c>
       <c r="L467" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M467" t="inlineStr">
@@ -23218,7 +23218,7 @@
       </c>
       <c r="L468" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M468" t="inlineStr">
@@ -23361,7 +23361,7 @@
       </c>
       <c r="L471" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M471" t="inlineStr">
@@ -23504,7 +23504,7 @@
       </c>
       <c r="L474" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M474" t="inlineStr">
@@ -23692,7 +23692,7 @@
       </c>
       <c r="L478" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M478" t="inlineStr">
@@ -23790,7 +23790,7 @@
       </c>
       <c r="L480" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
       <c r="M480" t="inlineStr">
@@ -23839,7 +23839,7 @@
       </c>
       <c r="L481" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M481" t="inlineStr">
@@ -24125,7 +24125,7 @@
       </c>
       <c r="L487" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M487" t="inlineStr">
@@ -24272,7 +24272,7 @@
       </c>
       <c r="L490" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
       <c r="M490" t="inlineStr">
@@ -24321,7 +24321,7 @@
       </c>
       <c r="L491" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M491" t="inlineStr">
@@ -24370,7 +24370,7 @@
       </c>
       <c r="L492" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M492" t="inlineStr">
@@ -24419,7 +24419,7 @@
       </c>
       <c r="L493" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M493" t="inlineStr">
@@ -24611,7 +24611,7 @@
       </c>
       <c r="L497" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M497" t="inlineStr">
@@ -30005,7 +30005,7 @@
       </c>
       <c r="L611" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M611" t="inlineStr">
@@ -34852,7 +34852,7 @@
       </c>
       <c r="L714" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M714" t="inlineStr">
@@ -34950,7 +34950,7 @@
       </c>
       <c r="L716" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M716" t="inlineStr">
@@ -35187,7 +35187,7 @@
       </c>
       <c r="L721" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M721" t="inlineStr">
@@ -35825,7 +35825,7 @@
       </c>
       <c r="L735" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M735" t="inlineStr">
@@ -36753,7 +36753,7 @@
       </c>
       <c r="L755" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M755" t="inlineStr">
@@ -36851,7 +36851,7 @@
       </c>
       <c r="L757" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
       <c r="M757" t="inlineStr">
@@ -36900,7 +36900,7 @@
       </c>
       <c r="L758" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M758" t="inlineStr">
@@ -38781,7 +38781,7 @@
       </c>
       <c r="L799" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M799" t="inlineStr">
@@ -38879,7 +38879,7 @@
       </c>
       <c r="L801" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M801" t="inlineStr">
@@ -39292,7 +39292,7 @@
       </c>
       <c r="L810" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M810" t="inlineStr">
@@ -39615,7 +39615,7 @@
       </c>
       <c r="L817" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M817" t="inlineStr">
@@ -39713,7 +39713,7 @@
       </c>
       <c r="L819" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M819" t="inlineStr">
@@ -40007,7 +40007,7 @@
       </c>
       <c r="L825" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
       <c r="M825" t="inlineStr">
@@ -40105,7 +40105,7 @@
       </c>
       <c r="L827" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="M827" t="inlineStr">
@@ -40154,7 +40154,7 @@
       </c>
       <c r="L828" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M828" t="inlineStr">
@@ -40248,7 +40248,7 @@
       </c>
       <c r="L830" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M830" t="inlineStr">
@@ -40346,7 +40346,7 @@
       </c>
       <c r="L832" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M832" t="inlineStr">
@@ -40726,7 +40726,7 @@
       </c>
       <c r="L840" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M840" t="inlineStr">
@@ -40873,7 +40873,7 @@
       </c>
       <c r="L843" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M843" t="inlineStr">
@@ -40922,7 +40922,7 @@
       </c>
       <c r="L844" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M844" t="inlineStr">
@@ -41020,7 +41020,7 @@
       </c>
       <c r="L846" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M846" t="inlineStr">
@@ -41069,7 +41069,7 @@
       </c>
       <c r="L847" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M847" t="inlineStr">
@@ -41216,7 +41216,7 @@
       </c>
       <c r="L850" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M850" t="inlineStr">
@@ -41408,7 +41408,7 @@
       </c>
       <c r="L854" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="M854" t="inlineStr">
@@ -41457,7 +41457,7 @@
       </c>
       <c r="L855" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M855" t="inlineStr">
@@ -41649,7 +41649,7 @@
       </c>
       <c r="L859" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="M859" t="inlineStr">
@@ -41743,7 +41743,7 @@
       </c>
       <c r="L861" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M861" t="inlineStr">
@@ -41841,7 +41841,7 @@
       </c>
       <c r="L863" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M863" t="inlineStr">
@@ -41890,7 +41890,7 @@
       </c>
       <c r="L864" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M864" t="inlineStr">
@@ -41988,7 +41988,7 @@
       </c>
       <c r="L866" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M866" t="inlineStr">
@@ -42037,7 +42037,7 @@
       </c>
       <c r="L867" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M867" t="inlineStr">
@@ -42135,7 +42135,7 @@
       </c>
       <c r="L869" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M869" t="inlineStr">
@@ -42184,7 +42184,7 @@
       </c>
       <c r="L870" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M870" t="inlineStr">
@@ -42282,7 +42282,7 @@
       </c>
       <c r="L872" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M872" t="inlineStr">
@@ -42331,7 +42331,7 @@
       </c>
       <c r="L873" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M873" t="inlineStr">
@@ -42429,7 +42429,7 @@
       </c>
       <c r="L875" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M875" t="inlineStr">
@@ -42478,7 +42478,7 @@
       </c>
       <c r="L876" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M876" t="inlineStr">
@@ -42576,7 +42576,7 @@
       </c>
       <c r="L878" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M878" t="inlineStr">
@@ -42625,7 +42625,7 @@
       </c>
       <c r="L879" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M879" t="inlineStr">
@@ -42723,7 +42723,7 @@
       </c>
       <c r="L881" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M881" t="inlineStr">
@@ -42772,7 +42772,7 @@
       </c>
       <c r="L882" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M882" t="inlineStr">
@@ -42870,7 +42870,7 @@
       </c>
       <c r="L884" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M884" t="inlineStr">
@@ -43017,7 +43017,7 @@
       </c>
       <c r="L887" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M887" t="inlineStr">
@@ -43066,7 +43066,7 @@
       </c>
       <c r="L888" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M888" t="inlineStr">
@@ -43164,7 +43164,7 @@
       </c>
       <c r="L890" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M890" t="inlineStr">
@@ -43213,7 +43213,7 @@
       </c>
       <c r="L891" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M891" t="inlineStr">
@@ -43311,7 +43311,7 @@
       </c>
       <c r="L893" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M893" t="inlineStr">
@@ -43540,7 +43540,7 @@
       </c>
       <c r="L898" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M898" t="inlineStr">
@@ -43638,7 +43638,7 @@
       </c>
       <c r="L900" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M900" t="inlineStr">
@@ -43687,7 +43687,7 @@
       </c>
       <c r="L901" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M901" t="inlineStr">
@@ -43785,7 +43785,7 @@
       </c>
       <c r="L903" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M903" t="inlineStr">
@@ -44259,7 +44259,7 @@
       </c>
       <c r="L913" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M913" t="inlineStr">
@@ -44357,7 +44357,7 @@
       </c>
       <c r="L915" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M915" t="inlineStr">
@@ -44455,7 +44455,7 @@
       </c>
       <c r="L917" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
       <c r="M917" t="inlineStr">
@@ -44553,7 +44553,7 @@
       </c>
       <c r="L919" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M919" t="inlineStr">
@@ -44696,7 +44696,7 @@
       </c>
       <c r="L922" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
       <c r="M922" t="inlineStr">
@@ -44794,7 +44794,7 @@
       </c>
       <c r="L924" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M924" t="inlineStr">
@@ -44990,7 +44990,7 @@
       </c>
       <c r="L928" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M928" t="inlineStr">
@@ -45088,7 +45088,7 @@
       </c>
       <c r="L930" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M930" t="inlineStr">
@@ -45231,7 +45231,7 @@
       </c>
       <c r="L933" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
       <c r="M933" t="inlineStr">
@@ -45329,7 +45329,7 @@
       </c>
       <c r="L935" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M935" t="inlineStr">
@@ -45472,7 +45472,7 @@
       </c>
       <c r="L938" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
       <c r="M938" t="inlineStr">
@@ -45570,7 +45570,7 @@
       </c>
       <c r="L940" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M940" t="inlineStr">
@@ -45709,7 +45709,7 @@
       </c>
       <c r="L943" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M943" t="inlineStr">
@@ -45807,7 +45807,7 @@
       </c>
       <c r="L945" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M945" t="inlineStr">
@@ -45856,7 +45856,7 @@
       </c>
       <c r="L946" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M946" t="inlineStr">
@@ -45954,7 +45954,7 @@
       </c>
       <c r="L948" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M948" t="inlineStr">
@@ -46003,7 +46003,7 @@
       </c>
       <c r="L949" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M949" t="inlineStr">
@@ -46101,7 +46101,7 @@
       </c>
       <c r="L951" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M951" t="inlineStr">
@@ -46199,7 +46199,7 @@
       </c>
       <c r="L953" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M953" t="inlineStr">
@@ -46297,7 +46297,7 @@
       </c>
       <c r="L955" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M955" t="inlineStr">
@@ -46346,7 +46346,7 @@
       </c>
       <c r="L956" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M956" t="inlineStr">
@@ -46575,7 +46575,7 @@
       </c>
       <c r="L961" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M961" t="inlineStr">
@@ -46673,7 +46673,7 @@
       </c>
       <c r="L963" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M963" t="inlineStr">
@@ -46812,7 +46812,7 @@
       </c>
       <c r="L966" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M966" t="inlineStr">
@@ -46910,7 +46910,7 @@
       </c>
       <c r="L968" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M968" t="inlineStr">
@@ -47151,7 +47151,7 @@
       </c>
       <c r="L973" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M973" t="inlineStr">
@@ -47249,7 +47249,7 @@
       </c>
       <c r="L975" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M975" t="inlineStr">
@@ -47298,7 +47298,7 @@
       </c>
       <c r="L976" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M976" t="inlineStr">
@@ -47396,7 +47396,7 @@
       </c>
       <c r="L978" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M978" t="inlineStr">
@@ -47494,7 +47494,7 @@
       </c>
       <c r="L980" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M980" t="inlineStr">
@@ -47543,7 +47543,7 @@
       </c>
       <c r="L981" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M981" t="inlineStr">
@@ -47641,7 +47641,7 @@
       </c>
       <c r="L983" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M983" t="inlineStr">
@@ -47690,7 +47690,7 @@
       </c>
       <c r="L984" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M984" t="inlineStr">
@@ -47788,7 +47788,7 @@
       </c>
       <c r="L986" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M986" t="inlineStr">
@@ -47837,7 +47837,7 @@
       </c>
       <c r="L987" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M987" t="inlineStr">
@@ -47935,7 +47935,7 @@
       </c>
       <c r="L989" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M989" t="inlineStr">
@@ -47984,7 +47984,7 @@
       </c>
       <c r="L990" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M990" t="inlineStr">
@@ -48082,7 +48082,7 @@
       </c>
       <c r="L992" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M992" t="inlineStr">
@@ -48131,7 +48131,7 @@
       </c>
       <c r="L993" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M993" t="inlineStr">
@@ -48229,7 +48229,7 @@
       </c>
       <c r="L995" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M995" t="inlineStr">
@@ -48327,7 +48327,7 @@
       </c>
       <c r="L997" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M997" t="inlineStr">
@@ -48376,7 +48376,7 @@
       </c>
       <c r="L998" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M998" t="inlineStr">
@@ -48425,7 +48425,7 @@
       </c>
       <c r="L999" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M999" t="inlineStr">
@@ -48523,7 +48523,7 @@
       </c>
       <c r="L1001" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1001" t="inlineStr">
@@ -48572,7 +48572,7 @@
       </c>
       <c r="L1002" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1002" t="inlineStr">
@@ -48670,7 +48670,7 @@
       </c>
       <c r="L1004" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
       <c r="M1004" t="inlineStr">
@@ -48719,7 +48719,7 @@
       </c>
       <c r="L1005" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1005" t="inlineStr">
@@ -48768,7 +48768,7 @@
       </c>
       <c r="L1006" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1006" t="inlineStr">
@@ -48866,7 +48866,7 @@
       </c>
       <c r="L1008" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1008" t="inlineStr">
@@ -48915,7 +48915,7 @@
       </c>
       <c r="L1009" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1009" t="inlineStr">
@@ -49013,7 +49013,7 @@
       </c>
       <c r="L1011" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1011" t="inlineStr">
@@ -49111,7 +49111,7 @@
       </c>
       <c r="L1013" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1013" t="inlineStr">
@@ -49209,7 +49209,7 @@
       </c>
       <c r="L1015" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1015" t="inlineStr">
@@ -49348,7 +49348,7 @@
       </c>
       <c r="L1018" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1018" t="inlineStr">
@@ -49446,7 +49446,7 @@
       </c>
       <c r="L1020" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1020" t="inlineStr">
@@ -49585,7 +49585,7 @@
       </c>
       <c r="L1023" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1023" t="inlineStr">
@@ -49683,7 +49683,7 @@
       </c>
       <c r="L1025" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1025" t="inlineStr">
@@ -49732,7 +49732,7 @@
       </c>
       <c r="L1026" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1026" t="inlineStr">
@@ -49781,7 +49781,7 @@
       </c>
       <c r="L1027" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1027" t="inlineStr">
@@ -49879,7 +49879,7 @@
       </c>
       <c r="L1029" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1029" t="inlineStr">
@@ -50071,7 +50071,7 @@
       </c>
       <c r="L1033" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1033" t="inlineStr">
@@ -50169,7 +50169,7 @@
       </c>
       <c r="L1035" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1035" t="inlineStr">
@@ -50316,7 +50316,7 @@
       </c>
       <c r="L1038" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1038" t="inlineStr">
@@ -50365,7 +50365,7 @@
       </c>
       <c r="L1039" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1039" t="inlineStr">
@@ -50463,7 +50463,7 @@
       </c>
       <c r="L1041" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1041" t="inlineStr">
@@ -50512,7 +50512,7 @@
       </c>
       <c r="L1042" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1042" t="inlineStr">
@@ -50610,7 +50610,7 @@
       </c>
       <c r="L1044" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1044" t="inlineStr">
@@ -50659,7 +50659,7 @@
       </c>
       <c r="L1045" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1045" t="inlineStr">
@@ -50757,7 +50757,7 @@
       </c>
       <c r="L1047" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1047" t="inlineStr">
@@ -50806,7 +50806,7 @@
       </c>
       <c r="L1048" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1048" t="inlineStr">
@@ -50953,7 +50953,7 @@
       </c>
       <c r="L1051" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1051" t="inlineStr">
@@ -51239,7 +51239,7 @@
       </c>
       <c r="L1057" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1057" t="inlineStr">
@@ -51288,7 +51288,7 @@
       </c>
       <c r="L1058" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1058" t="inlineStr">
@@ -51435,7 +51435,7 @@
       </c>
       <c r="L1061" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1061" t="inlineStr">
@@ -51578,7 +51578,7 @@
       </c>
       <c r="L1064" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1064" t="inlineStr">
@@ -51725,7 +51725,7 @@
       </c>
       <c r="L1067" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1067" t="inlineStr">
@@ -52539,7 +52539,7 @@
       </c>
       <c r="L1085" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1085" t="inlineStr">
@@ -52637,7 +52637,7 @@
       </c>
       <c r="L1087" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1087" t="inlineStr">
@@ -52825,7 +52825,7 @@
       </c>
       <c r="L1091" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1091" t="inlineStr">
@@ -52919,7 +52919,7 @@
       </c>
       <c r="L1093" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1093" t="inlineStr">
@@ -53017,7 +53017,7 @@
       </c>
       <c r="L1095" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1095" t="inlineStr">
@@ -53111,7 +53111,7 @@
       </c>
       <c r="L1097" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1097" t="inlineStr">
@@ -53160,7 +53160,7 @@
       </c>
       <c r="L1098" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1098" t="inlineStr">
@@ -53745,7 +53745,7 @@
       </c>
       <c r="L1111" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1111" t="inlineStr">
@@ -53843,7 +53843,7 @@
       </c>
       <c r="L1113" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1113" t="inlineStr">
@@ -53892,7 +53892,7 @@
       </c>
       <c r="L1114" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1114" t="inlineStr">
@@ -53990,7 +53990,7 @@
       </c>
       <c r="L1116" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1116" t="inlineStr">
@@ -54325,7 +54325,7 @@
       </c>
       <c r="L1123" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1123" t="inlineStr">
@@ -54423,7 +54423,7 @@
       </c>
       <c r="L1125" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1125" t="inlineStr">
@@ -54521,7 +54521,7 @@
       </c>
       <c r="L1127" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1127" t="inlineStr">
@@ -54709,7 +54709,7 @@
       </c>
       <c r="L1131" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1131" t="inlineStr">
@@ -54807,7 +54807,7 @@
       </c>
       <c r="L1133" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1133" t="inlineStr">
@@ -54946,7 +54946,7 @@
       </c>
       <c r="L1136" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1136" t="inlineStr">
@@ -55044,7 +55044,7 @@
       </c>
       <c r="L1138" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1138" t="inlineStr">
@@ -55093,7 +55093,7 @@
       </c>
       <c r="L1139" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1139" t="inlineStr">
@@ -55191,7 +55191,7 @@
       </c>
       <c r="L1141" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1141" t="inlineStr">
@@ -55240,7 +55240,7 @@
       </c>
       <c r="L1142" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1142" t="inlineStr">
@@ -55289,7 +55289,7 @@
       </c>
       <c r="L1143" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1143" t="inlineStr">
@@ -55338,7 +55338,7 @@
       </c>
       <c r="L1144" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1144" t="inlineStr">
@@ -55387,7 +55387,7 @@
       </c>
       <c r="L1145" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1145" t="inlineStr">
@@ -55710,7 +55710,7 @@
       </c>
       <c r="L1152" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1152" t="inlineStr">
@@ -55992,7 +55992,7 @@
       </c>
       <c r="L1158" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1158" t="inlineStr">
@@ -56090,7 +56090,7 @@
       </c>
       <c r="L1160" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1160" t="inlineStr">
@@ -56139,7 +56139,7 @@
       </c>
       <c r="L1161" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1161" t="inlineStr">
@@ -56237,7 +56237,7 @@
       </c>
       <c r="L1163" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1163" t="inlineStr">
@@ -56335,7 +56335,7 @@
       </c>
       <c r="L1165" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
       <c r="M1165" t="inlineStr">
@@ -56384,7 +56384,7 @@
       </c>
       <c r="L1166" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1166" t="inlineStr">
@@ -56433,7 +56433,7 @@
       </c>
       <c r="L1167" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1167" t="inlineStr">
@@ -56531,7 +56531,7 @@
       </c>
       <c r="L1169" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1169" t="inlineStr">
@@ -56580,7 +56580,7 @@
       </c>
       <c r="L1170" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1170" t="inlineStr">
@@ -56678,7 +56678,7 @@
       </c>
       <c r="L1172" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1172" t="inlineStr">
@@ -56776,7 +56776,7 @@
       </c>
       <c r="L1174" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1174" t="inlineStr">
@@ -56825,7 +56825,7 @@
       </c>
       <c r="L1175" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1175" t="inlineStr">
@@ -56919,7 +56919,7 @@
       </c>
       <c r="L1177" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1177" t="inlineStr">
@@ -57017,7 +57017,7 @@
       </c>
       <c r="L1179" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1179" t="inlineStr">
@@ -57512,7 +57512,7 @@
       </c>
       <c r="L1190" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1190" t="inlineStr">
@@ -57610,7 +57610,7 @@
       </c>
       <c r="L1192" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1192" t="inlineStr">
@@ -57798,7 +57798,7 @@
       </c>
       <c r="L1196" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1196" t="inlineStr">
@@ -57896,7 +57896,7 @@
       </c>
       <c r="L1198" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1198" t="inlineStr">
@@ -57945,7 +57945,7 @@
       </c>
       <c r="L1199" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1199" t="inlineStr">
@@ -58043,7 +58043,7 @@
       </c>
       <c r="L1201" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1201" t="inlineStr">
@@ -58092,7 +58092,7 @@
       </c>
       <c r="L1202" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1202" t="inlineStr">
@@ -58190,7 +58190,7 @@
       </c>
       <c r="L1204" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
       <c r="M1204" t="inlineStr">
@@ -58239,7 +58239,7 @@
       </c>
       <c r="L1205" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1205" t="inlineStr">
@@ -58480,7 +58480,7 @@
       </c>
       <c r="L1210" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1210" t="inlineStr">
@@ -58578,7 +58578,7 @@
       </c>
       <c r="L1212" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
       <c r="M1212" t="inlineStr">
@@ -58627,7 +58627,7 @@
       </c>
       <c r="L1213" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1213" t="inlineStr">
@@ -58725,7 +58725,7 @@
       </c>
       <c r="L1215" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M1215" t="inlineStr">
@@ -58774,7 +58774,7 @@
       </c>
       <c r="L1216" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1216" t="inlineStr">
@@ -58917,7 +58917,7 @@
       </c>
       <c r="L1219" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1219" t="inlineStr">
@@ -58966,7 +58966,7 @@
       </c>
       <c r="L1220" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1220" t="inlineStr">
@@ -59015,7 +59015,7 @@
       </c>
       <c r="L1221" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1221" t="inlineStr">
@@ -59064,7 +59064,7 @@
       </c>
       <c r="L1222" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1222" t="inlineStr">
@@ -59113,7 +59113,7 @@
       </c>
       <c r="L1223" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1223" t="inlineStr">
@@ -59256,7 +59256,7 @@
       </c>
       <c r="L1226" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1226" t="inlineStr">
@@ -59354,7 +59354,7 @@
       </c>
       <c r="L1228" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1228" t="inlineStr">
@@ -59722,7 +59722,7 @@
       </c>
       <c r="L1236" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1236" t="inlineStr">
@@ -59771,7 +59771,7 @@
       </c>
       <c r="L1237" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1237" t="inlineStr">
@@ -59869,7 +59869,7 @@
       </c>
       <c r="L1239" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1239" t="inlineStr">
@@ -60016,7 +60016,7 @@
       </c>
       <c r="L1242" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1242" t="inlineStr">
@@ -60114,7 +60114,7 @@
       </c>
       <c r="L1244" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1244" t="inlineStr">
@@ -60163,7 +60163,7 @@
       </c>
       <c r="L1245" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1245" t="inlineStr">
@@ -60261,7 +60261,7 @@
       </c>
       <c r="L1247" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1247" t="inlineStr">
@@ -60310,7 +60310,7 @@
       </c>
       <c r="L1248" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1248" t="inlineStr">
@@ -60408,7 +60408,7 @@
       </c>
       <c r="L1250" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1250" t="inlineStr">
@@ -60457,7 +60457,7 @@
       </c>
       <c r="L1251" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1251" t="inlineStr">
@@ -60555,7 +60555,7 @@
       </c>
       <c r="L1253" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1253" t="inlineStr">
@@ -60604,7 +60604,7 @@
       </c>
       <c r="L1254" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1254" t="inlineStr">
@@ -60702,7 +60702,7 @@
       </c>
       <c r="L1256" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1256" t="inlineStr">
@@ -60751,7 +60751,7 @@
       </c>
       <c r="L1257" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1257" t="inlineStr">
@@ -60849,7 +60849,7 @@
       </c>
       <c r="L1259" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1259" t="inlineStr">
@@ -60898,7 +60898,7 @@
       </c>
       <c r="L1260" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1260" t="inlineStr">
@@ -60996,7 +60996,7 @@
       </c>
       <c r="L1262" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1262" t="inlineStr">
@@ -61045,7 +61045,7 @@
       </c>
       <c r="L1263" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1263" t="inlineStr">
@@ -61143,7 +61143,7 @@
       </c>
       <c r="L1265" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1265" t="inlineStr">
@@ -61192,7 +61192,7 @@
       </c>
       <c r="L1266" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1266" t="inlineStr">
@@ -61290,7 +61290,7 @@
       </c>
       <c r="L1268" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1268" t="inlineStr">
@@ -61339,7 +61339,7 @@
       </c>
       <c r="L1269" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1269" t="inlineStr">
@@ -61437,7 +61437,7 @@
       </c>
       <c r="L1271" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1271" t="inlineStr">
@@ -61535,7 +61535,7 @@
       </c>
       <c r="L1273" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1273" t="inlineStr">
@@ -61584,7 +61584,7 @@
       </c>
       <c r="L1274" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1274" t="inlineStr">
@@ -61682,7 +61682,7 @@
       </c>
       <c r="L1276" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1276" t="inlineStr">
@@ -61870,7 +61870,7 @@
       </c>
       <c r="L1280" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="M1280" t="inlineStr">
@@ -61968,7 +61968,7 @@
       </c>
       <c r="L1282" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1282" t="inlineStr">
@@ -62017,7 +62017,7 @@
       </c>
       <c r="L1283" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1283" t="inlineStr">
@@ -62115,7 +62115,7 @@
       </c>
       <c r="L1285" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1285" t="inlineStr">
@@ -62213,7 +62213,7 @@
       </c>
       <c r="L1287" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1287" t="inlineStr">
@@ -62634,7 +62634,7 @@
       </c>
       <c r="L1296" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1296" t="inlineStr">
@@ -62777,7 +62777,7 @@
       </c>
       <c r="L1299" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1299" t="inlineStr">
@@ -63100,7 +63100,7 @@
       </c>
       <c r="L1306" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1306" t="inlineStr">
@@ -63198,7 +63198,7 @@
       </c>
       <c r="L1308" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1308" t="inlineStr">
@@ -63296,7 +63296,7 @@
       </c>
       <c r="L1310" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1310" t="inlineStr">
@@ -63570,7 +63570,7 @@
       </c>
       <c r="L1316" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1316" t="inlineStr">
@@ -63668,7 +63668,7 @@
       </c>
       <c r="L1318" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1318" t="inlineStr">
@@ -63766,7 +63766,7 @@
       </c>
       <c r="L1320" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1320" t="inlineStr">
@@ -63815,7 +63815,7 @@
       </c>
       <c r="L1321" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1321" t="inlineStr">
@@ -63913,7 +63913,7 @@
       </c>
       <c r="L1323" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1323" t="inlineStr">
@@ -64011,7 +64011,7 @@
       </c>
       <c r="L1325" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1325" t="inlineStr">
@@ -64109,7 +64109,7 @@
       </c>
       <c r="L1327" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1327" t="inlineStr">
@@ -64207,7 +64207,7 @@
       </c>
       <c r="L1329" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1329" t="inlineStr">
@@ -64305,7 +64305,7 @@
       </c>
       <c r="L1331" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1331" t="inlineStr">
@@ -64403,7 +64403,7 @@
       </c>
       <c r="L1333" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1333" t="inlineStr">
@@ -64501,7 +64501,7 @@
       </c>
       <c r="L1335" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1335" t="inlineStr">
@@ -64599,7 +64599,7 @@
       </c>
       <c r="L1337" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1337" t="inlineStr">
@@ -64697,7 +64697,7 @@
       </c>
       <c r="L1339" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1339" t="inlineStr">
@@ -64746,7 +64746,7 @@
       </c>
       <c r="L1340" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1340" t="inlineStr">
@@ -64844,7 +64844,7 @@
       </c>
       <c r="L1342" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1342" t="inlineStr">
@@ -64991,7 +64991,7 @@
       </c>
       <c r="L1345" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1345" t="inlineStr">
@@ -65089,7 +65089,7 @@
       </c>
       <c r="L1347" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
       <c r="M1347" t="inlineStr">
@@ -65138,7 +65138,7 @@
       </c>
       <c r="L1348" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1348" t="inlineStr">
@@ -65236,7 +65236,7 @@
       </c>
       <c r="L1350" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1350" t="inlineStr">
@@ -65424,7 +65424,7 @@
       </c>
       <c r="L1354" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1354" t="inlineStr">
@@ -65522,7 +65522,7 @@
       </c>
       <c r="L1356" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1356" t="inlineStr">
@@ -65571,7 +65571,7 @@
       </c>
       <c r="L1357" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1357" t="inlineStr">
@@ -65669,7 +65669,7 @@
       </c>
       <c r="L1359" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
       <c r="M1359" t="inlineStr">
@@ -65718,7 +65718,7 @@
       </c>
       <c r="L1360" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1360" t="inlineStr">
@@ -65767,7 +65767,7 @@
       </c>
       <c r="L1361" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1361" t="inlineStr">
@@ -65865,7 +65865,7 @@
       </c>
       <c r="L1363" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1363" t="inlineStr">
@@ -65914,7 +65914,7 @@
       </c>
       <c r="L1364" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1364" t="inlineStr">
@@ -66012,7 +66012,7 @@
       </c>
       <c r="L1366" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1366" t="inlineStr">
@@ -66110,7 +66110,7 @@
       </c>
       <c r="L1368" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1368" t="inlineStr">
@@ -66208,7 +66208,7 @@
       </c>
       <c r="L1370" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1370" t="inlineStr">
@@ -66306,7 +66306,7 @@
       </c>
       <c r="L1372" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1372" t="inlineStr">
@@ -66498,7 +66498,7 @@
       </c>
       <c r="L1376" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1376" t="inlineStr">
@@ -66596,7 +66596,7 @@
       </c>
       <c r="L1378" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1378" t="inlineStr">
@@ -66645,7 +66645,7 @@
       </c>
       <c r="L1379" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1379" t="inlineStr">
@@ -66788,7 +66788,7 @@
       </c>
       <c r="L1382" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1382" t="inlineStr">
@@ -66886,7 +66886,7 @@
       </c>
       <c r="L1384" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1384" t="inlineStr">
@@ -67033,7 +67033,7 @@
       </c>
       <c r="L1387" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1387" t="inlineStr">
@@ -67082,7 +67082,7 @@
       </c>
       <c r="L1388" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1388" t="inlineStr">
@@ -67180,7 +67180,7 @@
       </c>
       <c r="L1390" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1390" t="inlineStr">
@@ -67278,7 +67278,7 @@
       </c>
       <c r="L1392" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1392" t="inlineStr">
@@ -67376,7 +67376,7 @@
       </c>
       <c r="L1394" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
       <c r="M1394" t="inlineStr">
@@ -67519,7 +67519,7 @@
       </c>
       <c r="L1397" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1397" t="inlineStr">
@@ -67617,7 +67617,7 @@
       </c>
       <c r="L1399" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1399" t="inlineStr">
@@ -67666,7 +67666,7 @@
       </c>
       <c r="L1400" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1400" t="inlineStr">
@@ -67764,7 +67764,7 @@
       </c>
       <c r="L1402" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1402" t="inlineStr">
@@ -67952,7 +67952,7 @@
       </c>
       <c r="L1406" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
       <c r="M1406" t="inlineStr">
@@ -68001,7 +68001,7 @@
       </c>
       <c r="L1407" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
       <c r="M1407" t="inlineStr">
@@ -68050,7 +68050,7 @@
       </c>
       <c r="L1408" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1408" t="inlineStr">
@@ -68148,7 +68148,7 @@
       </c>
       <c r="L1410" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1410" t="inlineStr">
@@ -68340,7 +68340,7 @@
       </c>
       <c r="L1414" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1414" t="inlineStr">
@@ -68438,7 +68438,7 @@
       </c>
       <c r="L1416" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1416" t="inlineStr">
@@ -68536,7 +68536,7 @@
       </c>
       <c r="L1418" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1418" t="inlineStr">
@@ -68634,7 +68634,7 @@
       </c>
       <c r="L1420" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1420" t="inlineStr">
@@ -68732,7 +68732,7 @@
       </c>
       <c r="L1422" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1422" t="inlineStr">
@@ -68830,7 +68830,7 @@
       </c>
       <c r="L1424" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1424" t="inlineStr">
@@ -68928,7 +68928,7 @@
       </c>
       <c r="L1426" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1426" t="inlineStr">
@@ -68977,7 +68977,7 @@
       </c>
       <c r="L1427" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
       <c r="M1427" t="inlineStr">
@@ -69075,7 +69075,7 @@
       </c>
       <c r="L1429" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1429" t="inlineStr">
@@ -69222,7 +69222,7 @@
       </c>
       <c r="L1432" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
       <c r="M1432" t="inlineStr">

</xml_diff>